<commit_message>
#20161117 -> Penambahan implementation road
</commit_message>
<xml_diff>
--- a/PPT/Financial Analysis.xlsx
+++ b/PPT/Financial Analysis.xlsx
@@ -2,22 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffry Angtoni\git\RouterMaya\PPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine-PC\git\RouterMaya\PPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7170" windowHeight="4470" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7170" windowHeight="4470" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Cost" sheetId="1" r:id="rId1"/>
     <sheet name="Sales Scenario" sheetId="2" r:id="rId2"/>
     <sheet name="Sunk Cost Structure" sheetId="3" r:id="rId3"/>
     <sheet name="Break Even Point" sheetId="4" r:id="rId4"/>
+    <sheet name="Implementation Roadmap" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
   <si>
     <t>Office Space</t>
   </si>
@@ -177,16 +178,88 @@
   </si>
   <si>
     <t>Net Profit After Sunk Cost</t>
+  </si>
+  <si>
+    <t>Task/Month</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Web Development</t>
+  </si>
+  <si>
+    <t>Backend System Development</t>
+  </si>
+  <si>
+    <t>Technology Research</t>
+  </si>
+  <si>
+    <t>Dev to Production</t>
+  </si>
+  <si>
+    <t>Maintenance Phase</t>
+  </si>
+  <si>
+    <t>Quality Testing</t>
+  </si>
+  <si>
+    <t>Network Maintenance</t>
+  </si>
+  <si>
+    <t>Network Installation</t>
+  </si>
+  <si>
+    <t>Datacenter Installation</t>
+  </si>
+  <si>
+    <t>Year 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +292,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +323,72 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,18 +504,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,21 +528,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -406,65 +557,419 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="32" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -483,27 +988,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F17" totalsRowCount="1" headerRowDxfId="15" headerRowCellStyle="Accent3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F17" totalsRowCount="1" headerRowDxfId="41" headerRowCellStyle="Accent3">
   <autoFilter ref="B2:F16"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Quantity"/>
-    <tableColumn id="3" name="Cost/Month" dataDxfId="12"/>
-    <tableColumn id="4" name="Total Cost/Month" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="11"/>
-    <tableColumn id="5" name="Total Annual Cost" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="14"/>
+    <tableColumn id="3" name="Cost/Month" dataDxfId="40"/>
+    <tableColumn id="4" name="Total Cost/Month" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="5" name="Total Annual Cost" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:E11" totalsRowCount="1" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:E11" totalsRowCount="1" headerRowDxfId="35">
   <autoFilter ref="B2:E10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Quantity"/>
-    <tableColumn id="3" name="@" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Total" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="5">
+    <tableColumn id="3" name="@" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="4" name="Total" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>Table6[[#This Row],[@]]*Table6[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -516,13 +1021,57 @@
   <autoFilter ref="B2:G12"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Tahun Ke-"/>
-    <tableColumn id="2" name="Sunk Cost Remaining" dataDxfId="4"/>
-    <tableColumn id="3" name="Total Cost" dataDxfId="3"/>
-    <tableColumn id="4" name="Total Revenue" dataDxfId="2"/>
-    <tableColumn id="5" name="Profit" dataDxfId="0"/>
-    <tableColumn id="6" name="Net Profit After Sunk Cost" dataDxfId="1"/>
+    <tableColumn id="2" name="Sunk Cost Remaining" dataDxfId="30"/>
+    <tableColumn id="3" name="Total Cost" dataDxfId="29"/>
+    <tableColumn id="4" name="Total Revenue" dataDxfId="28"/>
+    <tableColumn id="5" name="Profit" dataDxfId="27"/>
+    <tableColumn id="6" name="Net Profit After Sunk Cost" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:N12" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="B3:N12"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Task/Month"/>
+    <tableColumn id="2" name="1" dataDxfId="24"/>
+    <tableColumn id="3" name="2" dataDxfId="23"/>
+    <tableColumn id="4" name="3" dataDxfId="22"/>
+    <tableColumn id="5" name="4" dataDxfId="21"/>
+    <tableColumn id="6" name="5" dataDxfId="20"/>
+    <tableColumn id="7" name="6" dataDxfId="19"/>
+    <tableColumn id="8" name="7" dataDxfId="18"/>
+    <tableColumn id="9" name="8" dataDxfId="17"/>
+    <tableColumn id="10" name="9" dataDxfId="16"/>
+    <tableColumn id="11" name="10" dataDxfId="15"/>
+    <tableColumn id="12" name="11" dataDxfId="14"/>
+    <tableColumn id="13" name="12" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B15:N24" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="B15:N24"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Task/Month"/>
+    <tableColumn id="2" name="1" dataDxfId="11"/>
+    <tableColumn id="3" name="2" dataDxfId="10"/>
+    <tableColumn id="4" name="3" dataDxfId="9"/>
+    <tableColumn id="5" name="4" dataDxfId="8"/>
+    <tableColumn id="6" name="5" dataDxfId="7"/>
+    <tableColumn id="7" name="6" dataDxfId="6"/>
+    <tableColumn id="8" name="7" dataDxfId="5"/>
+    <tableColumn id="9" name="8" dataDxfId="4"/>
+    <tableColumn id="10" name="9" dataDxfId="3"/>
+    <tableColumn id="11" name="10" dataDxfId="2"/>
+    <tableColumn id="12" name="11" dataDxfId="1"/>
+    <tableColumn id="13" name="12" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -791,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1135,799 +1684,799 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="7" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="23"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="29"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="11" t="s">
+      <c r="I3" s="30"/>
+      <c r="J3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="16">
         <f>$C21*$B$18</f>
         <v>30000000</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="16">
         <f>$D21*$B$18</f>
         <v>15000000</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="16">
         <f>$E21*$B$18</f>
         <v>26400000</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="16">
         <f>$F21*$B$18</f>
         <v>8400000</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <f>$G21*$B$18</f>
         <v>48000000</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="16">
         <f>$H21*$B$18</f>
         <v>120000000</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="17">
         <f>SUM(C4:H4)</f>
         <v>247800000</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="13">
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="16">
         <f t="shared" ref="C5:C13" si="0">$C22*$B$18</f>
         <v>33000000</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <f t="shared" ref="D5:D13" si="1">$D22*$B$18</f>
         <v>17400000</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="16">
         <f t="shared" ref="E5:E13" si="2">$E22*$B$18</f>
         <v>30000000</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="16">
         <f t="shared" ref="F5:F13" si="3">$F22*$B$18</f>
         <v>10800000</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <f t="shared" ref="G5:G13" si="4">$G22*$B$18</f>
         <v>60000000</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="16">
         <f t="shared" ref="H5:H13" si="5">$H22*$B$18</f>
         <v>156000000</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="17">
         <f t="shared" ref="I5:I13" si="6">SUM(C5:H5)</f>
         <v>307200000</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="18">
         <f>(($C5-$C$4)/$C$4)</f>
         <v>0.1</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="18">
         <f>(($D5-$D$4)/$D$4)</f>
         <v>0.16</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="18">
         <f>(($E5-$E$4)/$E$4)</f>
         <v>0.13636363636363635</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="18">
         <f>(($F5-$F$4)/$F$4)</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="18">
         <f>(($G5-$G$4)/$G$4)</f>
         <v>0.25</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="18">
         <f>(($H5-$H$4)/$H$4)</f>
         <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="16">
         <f t="shared" si="0"/>
         <v>36000000</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <f t="shared" si="1"/>
         <v>19200000</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="16">
         <f t="shared" si="2"/>
         <v>31500000</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="16">
         <f t="shared" si="3"/>
         <v>11400000</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <f t="shared" si="4"/>
         <v>67800000</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="16">
         <f t="shared" si="5"/>
         <v>174300000</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="17">
         <f t="shared" si="6"/>
         <v>340200000</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="18">
         <f t="shared" ref="J6:J13" si="7">(($C6-$C$4)/$C$4)</f>
         <v>0.2</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="18">
         <f t="shared" ref="K6:K13" si="8">(($D6-$D$4)/$D$4)</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="18">
         <f t="shared" ref="L6:L13" si="9">(($E6-$E$4)/$E$4)</f>
         <v>0.19318181818181818</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="18">
         <f t="shared" ref="M6:M13" si="10">(($F6-$F$4)/$F$4)</f>
         <v>0.35714285714285715</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="18">
         <f t="shared" ref="N6:N13" si="11">(($G6-$G$4)/$G$4)</f>
         <v>0.41249999999999998</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="18">
         <f t="shared" ref="O6:O13" si="12">(($H6-$H$4)/$H$4)</f>
         <v>0.45250000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="16">
         <f t="shared" si="0"/>
         <v>39000000</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="16">
         <f t="shared" si="1"/>
         <v>22200000</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="16">
         <f t="shared" si="2"/>
         <v>33060000</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="16">
         <f t="shared" si="3"/>
         <v>15000000</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="16">
         <f t="shared" si="4"/>
         <v>72000000</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="16">
         <f t="shared" si="5"/>
         <v>187824000</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="17">
         <f t="shared" si="6"/>
         <v>369084000</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="18">
         <f t="shared" si="7"/>
         <v>0.3</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="18">
         <f t="shared" si="8"/>
         <v>0.48</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="18">
         <f t="shared" si="9"/>
         <v>0.25227272727272726</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="18">
         <f t="shared" si="10"/>
         <v>0.7857142857142857</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="18">
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="18">
         <f t="shared" si="12"/>
         <v>0.56520000000000004</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="16">
         <f t="shared" si="0"/>
         <v>42000000</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="16">
         <f t="shared" si="1"/>
         <v>31200000</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="16">
         <f t="shared" si="2"/>
         <v>38400000</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="16">
         <f t="shared" si="3"/>
         <v>18000000</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <f t="shared" si="4"/>
         <v>75000000</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="16">
         <f t="shared" si="5"/>
         <v>196200000</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="17">
         <f t="shared" si="6"/>
         <v>400800000</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="18">
         <f t="shared" si="7"/>
         <v>0.4</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="18">
         <f t="shared" si="8"/>
         <v>1.08</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="18">
         <f t="shared" si="9"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="18">
         <f t="shared" si="10"/>
         <v>1.1428571428571428</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="18">
         <f t="shared" si="11"/>
         <v>0.5625</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8" s="18">
         <f t="shared" si="12"/>
         <v>0.63500000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="13">
+      <c r="B9" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="16">
         <f t="shared" si="0"/>
         <v>42600000</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="16">
         <f t="shared" si="1"/>
         <v>31800000</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="16">
         <f t="shared" si="2"/>
         <v>39000000</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="16">
         <f t="shared" si="3"/>
         <v>19800000</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="16">
         <f t="shared" si="4"/>
         <v>78000000</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="16">
         <f t="shared" si="5"/>
         <v>200400000</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="17">
         <f t="shared" si="6"/>
         <v>411600000</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="18">
         <f t="shared" si="7"/>
         <v>0.42</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="18">
         <f t="shared" si="8"/>
         <v>1.1200000000000001</v>
       </c>
-      <c r="L9" s="24">
+      <c r="L9" s="18">
         <f t="shared" si="9"/>
         <v>0.47727272727272729</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="18">
         <f t="shared" si="10"/>
         <v>1.3571428571428572</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="18">
         <f t="shared" si="11"/>
         <v>0.625</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="18">
         <f t="shared" si="12"/>
         <v>0.67</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
+      <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="16">
         <f t="shared" si="0"/>
         <v>45000000</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="16">
         <f t="shared" si="1"/>
         <v>34200000</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="16">
         <f t="shared" si="2"/>
         <v>41400000</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="16">
         <f t="shared" si="3"/>
         <v>21420000</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="16">
         <f t="shared" si="4"/>
         <v>78600000</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="16">
         <f t="shared" si="5"/>
         <v>203424000</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="17">
         <f t="shared" si="6"/>
         <v>424044000</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="18">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K10" s="18">
         <f t="shared" si="8"/>
         <v>1.28</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="18">
         <f t="shared" si="9"/>
         <v>0.56818181818181823</v>
       </c>
-      <c r="M10" s="24">
+      <c r="M10" s="18">
         <f t="shared" si="10"/>
         <v>1.55</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="18">
         <f t="shared" si="11"/>
         <v>0.63749999999999996</v>
       </c>
-      <c r="O10" s="24">
+      <c r="O10" s="18">
         <f t="shared" si="12"/>
         <v>0.69520000000000004</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
+      <c r="B11" s="10">
         <v>8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="16">
         <f t="shared" si="0"/>
         <v>47400000</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="16">
         <f t="shared" si="1"/>
         <v>35580000</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="16">
         <f t="shared" si="2"/>
         <v>42780000</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="16">
         <f t="shared" si="3"/>
         <v>23040000</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="16">
         <f t="shared" si="4"/>
         <v>79860000</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="16">
         <f t="shared" si="5"/>
         <v>207000000</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="17">
         <f t="shared" si="6"/>
         <v>435660000</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="18">
         <f t="shared" si="7"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="18">
         <f t="shared" si="8"/>
         <v>1.3720000000000001</v>
       </c>
-      <c r="L11" s="24">
+      <c r="L11" s="18">
         <f t="shared" si="9"/>
         <v>0.62045454545454548</v>
       </c>
-      <c r="M11" s="24">
+      <c r="M11" s="18">
         <f t="shared" si="10"/>
         <v>1.7428571428571429</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="18">
         <f t="shared" si="11"/>
         <v>0.66374999999999995</v>
       </c>
-      <c r="O11" s="24">
+      <c r="O11" s="18">
         <f t="shared" si="12"/>
         <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
+      <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="16">
         <f t="shared" si="0"/>
         <v>48696000</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="16">
         <f t="shared" si="1"/>
         <v>37824000</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="16">
         <f t="shared" si="2"/>
         <v>44400000</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="16">
         <f t="shared" si="3"/>
         <v>25500000</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="16">
         <f t="shared" si="4"/>
         <v>82200000</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="16">
         <f t="shared" si="5"/>
         <v>210300000</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="17">
         <f t="shared" si="6"/>
         <v>448920000</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="18">
         <f t="shared" si="7"/>
         <v>0.62319999999999998</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="18">
         <f t="shared" si="8"/>
         <v>1.5216000000000001</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="18">
         <f t="shared" si="9"/>
         <v>0.68181818181818177</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="18">
         <f t="shared" si="10"/>
         <v>2.0357142857142856</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="18">
         <f t="shared" si="11"/>
         <v>0.71250000000000002</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="18">
         <f t="shared" si="12"/>
         <v>0.75249999999999995</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="B13" s="10">
         <v>10</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="16">
         <f t="shared" si="0"/>
         <v>51000000</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="16">
         <f t="shared" si="1"/>
         <v>42300000</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="16">
         <f t="shared" si="2"/>
         <v>48000000</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="16">
         <f t="shared" si="3"/>
         <v>30540000</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="16">
         <f t="shared" si="4"/>
         <v>84600000</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="16">
         <f t="shared" si="5"/>
         <v>217500000</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="17">
         <f t="shared" si="6"/>
         <v>473940000</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="18">
         <f t="shared" si="7"/>
         <v>0.7</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="18">
         <f t="shared" si="8"/>
         <v>1.82</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="18">
         <f t="shared" si="9"/>
         <v>0.81818181818181823</v>
       </c>
-      <c r="M13" s="24">
+      <c r="M13" s="18">
         <f t="shared" si="10"/>
         <v>2.6357142857142857</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="18">
         <f t="shared" si="11"/>
         <v>0.76249999999999996</v>
       </c>
-      <c r="O13" s="24">
+      <c r="O13" s="18">
         <f t="shared" si="12"/>
         <v>0.8125</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="25" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="20">
         <f>SUM(I4:I13)</f>
         <v>3859248000</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
+      <c r="B18" s="13">
         <v>12</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="7" t="s">
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="33"/>
+      <c r="C20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="12">
+      <c r="B21" s="9">
         <v>1</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="16">
         <v>2500000</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="16">
         <v>1250000</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="16">
         <v>2200000</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="16">
         <v>700000</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="16">
         <v>4000000</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="16">
         <v>10000000</v>
       </c>
       <c r="I21" s="5"/>
@@ -1938,25 +2487,25 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="13">
+      <c r="B22" s="10">
         <v>2</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="17">
         <v>2750000</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="17">
         <v>1450000</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="17">
         <v>2500000</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="17">
         <v>900000</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="17">
         <v>5000000</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="17">
         <v>13000000</v>
       </c>
       <c r="I22" s="6"/>
@@ -1967,25 +2516,25 @@
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="12">
+      <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="17">
         <v>3000000</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="17">
         <v>1600000</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="17">
         <v>2625000</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="17">
         <v>950000</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="17">
         <v>5650000</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="17">
         <v>14525000</v>
       </c>
       <c r="I23" s="6"/>
@@ -1996,25 +2545,25 @@
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
+      <c r="B24" s="10">
         <v>4</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="17">
         <v>3250000</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="17">
         <v>1850000</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="17">
         <v>2755000</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="17">
         <v>1250000</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="17">
         <v>6000000</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="17">
         <v>15652000</v>
       </c>
       <c r="I24" s="6"/>
@@ -2025,25 +2574,25 @@
       <c r="N24" s="6"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
+      <c r="B25" s="9">
         <v>5</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="17">
         <v>3500000</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="17">
         <v>2600000</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="17">
         <v>3200000</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="17">
         <v>1500000</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="17">
         <v>6250000</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="17">
         <v>16350000</v>
       </c>
       <c r="I25" s="6"/>
@@ -2054,25 +2603,25 @@
       <c r="N25" s="6"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="13">
+      <c r="B26" s="10">
         <v>6</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="17">
         <v>3550000</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="17">
         <v>2650000</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="17">
         <v>3250000</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="17">
         <v>1650000</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="17">
         <v>6500000</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="17">
         <v>16700000</v>
       </c>
       <c r="I26" s="6"/>
@@ -2083,25 +2632,25 @@
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="12">
+      <c r="B27" s="9">
         <v>7</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="17">
         <v>3750000</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="17">
         <v>2850000</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="17">
         <v>3450000</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="17">
         <v>1785000</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="17">
         <v>6550000</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="17">
         <v>16952000</v>
       </c>
       <c r="I27" s="6"/>
@@ -2112,25 +2661,25 @@
       <c r="N27" s="6"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="13">
+      <c r="B28" s="10">
         <v>8</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="17">
         <v>3950000</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="17">
         <v>2965000</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="17">
         <v>3565000</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="17">
         <v>1920000</v>
       </c>
-      <c r="G28" s="20">
+      <c r="G28" s="17">
         <v>6655000</v>
       </c>
-      <c r="H28" s="20">
+      <c r="H28" s="17">
         <v>17250000</v>
       </c>
       <c r="I28" s="6"/>
@@ -2141,25 +2690,25 @@
       <c r="N28" s="6"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="12">
+      <c r="B29" s="9">
         <v>9</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="17">
         <v>4058000</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="17">
         <v>3152000</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="17">
         <v>3700000</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="17">
         <v>2125000</v>
       </c>
-      <c r="G29" s="20">
+      <c r="G29" s="17">
         <v>6850000</v>
       </c>
-      <c r="H29" s="20">
+      <c r="H29" s="17">
         <v>17525000</v>
       </c>
       <c r="I29" s="6"/>
@@ -2170,25 +2719,25 @@
       <c r="N29" s="6"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="13">
+      <c r="B30" s="10">
         <v>10</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="17">
         <v>4250000</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="17">
         <v>3525000</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="17">
         <v>4000000</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="17">
         <v>2545000</v>
       </c>
-      <c r="G30" s="20">
+      <c r="G30" s="17">
         <v>7050000</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H30" s="17">
         <v>18125000</v>
       </c>
       <c r="I30" s="6"/>
@@ -2199,345 +2748,348 @@
       <c r="N30" s="6"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="9" t="s">
+      <c r="D33" s="32"/>
+      <c r="E33" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="F33" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="10" t="s">
+      <c r="B34" s="30"/>
+      <c r="C34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="11" t="s">
+      <c r="E34" s="34"/>
+      <c r="F34" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="12">
+      <c r="B35" s="9">
         <v>1</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="16">
         <f>$I4</f>
         <v>247800000</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="16">
         <v>76250000</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="17">
         <f>SUM(C35,D35)</f>
         <v>324050000</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F35" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G35" s="18" t="s">
+      <c r="G35" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="13">
+      <c r="B36" s="10">
         <v>2</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="16">
         <f t="shared" ref="C36:C44" si="13">$I5</f>
         <v>307200000</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="16">
         <v>92252000</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="17">
         <f t="shared" ref="E36:E44" si="14">SUM(C36,D36)</f>
         <v>399452000</v>
       </c>
-      <c r="F36" s="24">
+      <c r="F36" s="18">
         <f>($C36-$C35)/$C35</f>
         <v>0.23970944309927361</v>
       </c>
-      <c r="G36" s="24">
+      <c r="G36" s="18">
         <f>($D36-$D35)/$D35</f>
         <v>0.20986229508196722</v>
       </c>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="12">
+      <c r="B37" s="9">
         <v>3</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="16">
         <f t="shared" si="13"/>
         <v>340200000</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="16">
         <v>95000000</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="17">
         <f t="shared" si="14"/>
         <v>435200000</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F37" s="18">
         <f t="shared" ref="F37:F44" si="15">($C37-$C36)/$C36</f>
         <v>0.107421875</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="18">
         <f>($D37-$D36)/$D36</f>
         <v>2.9787972076486147E-2</v>
       </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="13">
+      <c r="B38" s="10">
         <v>4</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="16">
         <f t="shared" si="13"/>
         <v>369084000</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D38" s="16">
         <v>98152000</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="17">
         <f t="shared" si="14"/>
         <v>467236000</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F38" s="18">
         <f>($C38-$C37)/$C37</f>
         <v>8.4902998236331573E-2</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="18">
         <f>($D38-$D37)/$D37</f>
         <v>3.3178947368421051E-2</v>
       </c>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="12">
+      <c r="B39" s="9">
         <v>5</v>
       </c>
-      <c r="C39" s="19">
+      <c r="C39" s="16">
         <f t="shared" si="13"/>
         <v>400800000</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D39" s="16">
         <v>100545000</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E39" s="17">
         <f t="shared" si="14"/>
         <v>501345000</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="18">
         <f>($C39-$C38)/$C38</f>
         <v>8.5931657833989011E-2</v>
       </c>
-      <c r="G39" s="24">
-        <f t="shared" ref="G37:G44" si="16">($D39-$D38)/$D38</f>
+      <c r="G39" s="18">
+        <f t="shared" ref="G39:G44" si="16">($D39-$D38)/$D38</f>
         <v>2.4380552612274838E-2</v>
       </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="13">
+      <c r="B40" s="10">
         <v>6</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C40" s="16">
         <f t="shared" si="13"/>
         <v>411600000</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="16">
         <v>101205000</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="17">
         <f t="shared" si="14"/>
         <v>512805000</v>
       </c>
-      <c r="F40" s="24">
+      <c r="F40" s="18">
         <f t="shared" si="15"/>
         <v>2.6946107784431138E-2</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="18">
         <f>($D40-$D39)/$D39</f>
         <v>6.5642249738922867E-3</v>
       </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="12">
+      <c r="B41" s="9">
         <v>7</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="16">
         <f t="shared" si="13"/>
         <v>424044000</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D41" s="16">
         <v>102000000</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="17">
         <f t="shared" si="14"/>
         <v>526044000</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="18">
         <f>($C41-$C40)/$C40</f>
         <v>3.0233236151603497E-2</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="18">
         <f t="shared" si="16"/>
         <v>7.8553431154587232E-3</v>
       </c>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="13">
+      <c r="B42" s="10">
         <v>8</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="16">
         <f t="shared" si="13"/>
         <v>435660000</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="16">
         <v>110250000</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="17">
         <f t="shared" si="14"/>
         <v>545910000</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="18">
         <f t="shared" si="15"/>
         <v>2.7393383705464527E-2</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="18">
         <f t="shared" si="16"/>
         <v>8.0882352941176475E-2</v>
       </c>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="12">
+      <c r="B43" s="9">
         <v>9</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C43" s="16">
         <f t="shared" si="13"/>
         <v>448920000</v>
       </c>
-      <c r="D43" s="19">
+      <c r="D43" s="16">
         <v>116585000</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="17">
         <f t="shared" si="14"/>
         <v>565505000</v>
       </c>
-      <c r="F43" s="24">
+      <c r="F43" s="18">
         <f t="shared" si="15"/>
         <v>3.0436578983611073E-2</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="18">
         <f t="shared" si="16"/>
         <v>5.7460317460317462E-2</v>
       </c>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="13">
+      <c r="B44" s="10">
         <v>10</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C44" s="16">
         <f t="shared" si="13"/>
         <v>473940000</v>
       </c>
-      <c r="D44" s="19">
+      <c r="D44" s="16">
         <v>120000000</v>
       </c>
-      <c r="E44" s="20">
+      <c r="E44" s="17">
         <f t="shared" si="14"/>
         <v>593940000</v>
       </c>
-      <c r="F44" s="24">
+      <c r="F44" s="18">
         <f t="shared" si="15"/>
         <v>5.5733761026463512E-2</v>
       </c>
-      <c r="G44" s="24">
+      <c r="G44" s="18">
         <f t="shared" si="16"/>
         <v>2.9291932924475704E-2</v>
       </c>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="25" t="s">
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="26">
+      <c r="E45" s="20">
         <f>SUM(E35:E44)</f>
         <v>4871487000</v>
       </c>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I19:N19"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="C33:D33"/>
@@ -2546,9 +3098,6 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="I19:N19"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2729,8 +3278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,7 +3321,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="36">
+      <c r="F3" s="27">
         <v>324050000</v>
       </c>
       <c r="G3" s="4"/>
@@ -2784,7 +3333,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="36">
+      <c r="F4" s="27">
         <v>399452000</v>
       </c>
       <c r="G4" s="4"/>
@@ -2796,7 +3345,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="36">
+      <c r="F5" s="27">
         <v>435200000</v>
       </c>
       <c r="G5" s="4"/>
@@ -2808,7 +3357,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="36">
+      <c r="F6" s="27">
         <v>467236000</v>
       </c>
       <c r="G6" s="4"/>
@@ -2820,7 +3369,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="36">
+      <c r="F7" s="27">
         <v>501345000</v>
       </c>
       <c r="G7" s="4"/>
@@ -2832,7 +3381,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="36">
+      <c r="F8" s="27">
         <v>512805000</v>
       </c>
       <c r="G8" s="4"/>
@@ -2844,7 +3393,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="36">
+      <c r="F9" s="27">
         <v>526044000</v>
       </c>
       <c r="G9" s="4"/>
@@ -2856,7 +3405,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="36">
+      <c r="F10" s="27">
         <v>545910000</v>
       </c>
       <c r="G10" s="4"/>
@@ -2868,7 +3417,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="36">
+      <c r="F11" s="27">
         <v>565505000</v>
       </c>
       <c r="G11" s="4"/>
@@ -2880,7 +3429,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="36">
+      <c r="F12" s="27">
         <v>593940000</v>
       </c>
       <c r="G12" s="4"/>
@@ -2891,4 +3440,454 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="49"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="49"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="59"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="49"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="59"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="59"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="57"/>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="48"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="50"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="50"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="49"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="49"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="49"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="59"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="49"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="59"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="49"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="59"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B14:N14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#20161117 -> Break Even
</commit_message>
<xml_diff>
--- a/PPT/Financial Analysis.xlsx
+++ b/PPT/Financial Analysis.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine-PC\git\RouterMaya\PPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffry Angtoni\git\RouterMaya\PPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7170" windowHeight="4470" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7170" windowHeight="4470" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Cost" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Break Even Point" sheetId="4" r:id="rId4"/>
     <sheet name="Implementation Roadmap" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t>Office Space</t>
   </si>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
   </numFmts>
@@ -493,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,36 +542,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -596,12 +566,64 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -939,28 +961,7 @@
       <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
@@ -994,21 +995,21 @@
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Quantity"/>
     <tableColumn id="3" name="Cost/Month" dataDxfId="40"/>
-    <tableColumn id="4" name="Total Cost/Month" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="5" name="Total Annual Cost" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="4" name="Total Cost/Month" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="6"/>
+    <tableColumn id="5" name="Total Annual Cost" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="5"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:E11" totalsRowCount="1" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:E11" totalsRowCount="1" headerRowDxfId="37">
   <autoFilter ref="B2:E10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Quantity"/>
-    <tableColumn id="3" name="@" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="4" name="Total" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
+    <tableColumn id="3" name="@" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="4" name="Total" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33">
       <calculatedColumnFormula>Table6[[#This Row],[@]]*Table6[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1021,55 +1022,59 @@
   <autoFilter ref="B2:G12"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Tahun Ke-"/>
-    <tableColumn id="2" name="Sunk Cost Remaining" dataDxfId="30"/>
-    <tableColumn id="3" name="Total Cost" dataDxfId="29"/>
-    <tableColumn id="4" name="Total Revenue" dataDxfId="28"/>
-    <tableColumn id="5" name="Profit" dataDxfId="27"/>
-    <tableColumn id="6" name="Net Profit After Sunk Cost" dataDxfId="26"/>
+    <tableColumn id="2" name="Sunk Cost Remaining" dataDxfId="4">
+      <calculatedColumnFormula>SUBTOTAL(109,Table6[Total])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Total Cost" dataDxfId="3"/>
+    <tableColumn id="4" name="Total Revenue" dataDxfId="1"/>
+    <tableColumn id="5" name="Profit" dataDxfId="0">
+      <calculatedColumnFormula>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Net Profit After Sunk Cost" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:N12" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:N12" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="B3:N12"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Task/Month"/>
-    <tableColumn id="2" name="1" dataDxfId="24"/>
-    <tableColumn id="3" name="2" dataDxfId="23"/>
-    <tableColumn id="4" name="3" dataDxfId="22"/>
-    <tableColumn id="5" name="4" dataDxfId="21"/>
-    <tableColumn id="6" name="5" dataDxfId="20"/>
-    <tableColumn id="7" name="6" dataDxfId="19"/>
-    <tableColumn id="8" name="7" dataDxfId="18"/>
-    <tableColumn id="9" name="8" dataDxfId="17"/>
-    <tableColumn id="10" name="9" dataDxfId="16"/>
-    <tableColumn id="11" name="10" dataDxfId="15"/>
-    <tableColumn id="12" name="11" dataDxfId="14"/>
-    <tableColumn id="13" name="12" dataDxfId="13"/>
+    <tableColumn id="2" name="1" dataDxfId="31"/>
+    <tableColumn id="3" name="2" dataDxfId="30"/>
+    <tableColumn id="4" name="3" dataDxfId="29"/>
+    <tableColumn id="5" name="4" dataDxfId="28"/>
+    <tableColumn id="6" name="5" dataDxfId="27"/>
+    <tableColumn id="7" name="6" dataDxfId="26"/>
+    <tableColumn id="8" name="7" dataDxfId="25"/>
+    <tableColumn id="9" name="8" dataDxfId="24"/>
+    <tableColumn id="10" name="9" dataDxfId="23"/>
+    <tableColumn id="11" name="10" dataDxfId="22"/>
+    <tableColumn id="12" name="11" dataDxfId="21"/>
+    <tableColumn id="13" name="12" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B15:N24" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B15:N24" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="B15:N24"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Task/Month"/>
-    <tableColumn id="2" name="1" dataDxfId="11"/>
-    <tableColumn id="3" name="2" dataDxfId="10"/>
-    <tableColumn id="4" name="3" dataDxfId="9"/>
-    <tableColumn id="5" name="4" dataDxfId="8"/>
-    <tableColumn id="6" name="5" dataDxfId="7"/>
-    <tableColumn id="7" name="6" dataDxfId="6"/>
-    <tableColumn id="8" name="7" dataDxfId="5"/>
-    <tableColumn id="9" name="8" dataDxfId="4"/>
-    <tableColumn id="10" name="9" dataDxfId="3"/>
-    <tableColumn id="11" name="10" dataDxfId="2"/>
-    <tableColumn id="12" name="11" dataDxfId="1"/>
-    <tableColumn id="13" name="12" dataDxfId="0"/>
+    <tableColumn id="2" name="1" dataDxfId="18"/>
+    <tableColumn id="3" name="2" dataDxfId="17"/>
+    <tableColumn id="4" name="3" dataDxfId="16"/>
+    <tableColumn id="5" name="4" dataDxfId="15"/>
+    <tableColumn id="6" name="5" dataDxfId="14"/>
+    <tableColumn id="7" name="6" dataDxfId="13"/>
+    <tableColumn id="8" name="7" dataDxfId="12"/>
+    <tableColumn id="9" name="8" dataDxfId="11"/>
+    <tableColumn id="10" name="9" dataDxfId="10"/>
+    <tableColumn id="11" name="10" dataDxfId="9"/>
+    <tableColumn id="12" name="11" dataDxfId="8"/>
+    <tableColumn id="13" name="12" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1341,7 +1346,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,15 +1383,15 @@
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>7000000</v>
+        <v>6000000</v>
       </c>
       <c r="E3" s="4">
         <f>$C3*$D3</f>
-        <v>7000000</v>
+        <v>6000000</v>
       </c>
       <c r="F3" s="4">
         <f>$E3*12</f>
-        <v>84000000</v>
+        <v>72000000</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1397,15 +1402,15 @@
         <v>1</v>
       </c>
       <c r="D4" s="4">
-        <v>3000000</v>
+        <v>1750000</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E16" si="0">$C4*$D4</f>
-        <v>3000000</v>
+        <v>1750000</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" ref="F4:F16" si="1">$E4*12</f>
-        <v>36000000</v>
+        <v>21000000</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1451,18 +1456,18 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>5600000</v>
+        <v>4000000</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>33600000</v>
+        <v>12000000</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="1"/>
-        <v>403200000</v>
+        <v>144000000</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1473,15 +1478,15 @@
         <v>2</v>
       </c>
       <c r="D8" s="4">
-        <v>6000000</v>
+        <v>5000000</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>12000000</v>
+        <v>10000000</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="1"/>
-        <v>144000000</v>
+        <v>120000000</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1603,18 +1608,18 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4">
-        <v>12000000</v>
+        <v>7000000</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>36000000</v>
+        <v>14000000</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="1"/>
-        <v>432000000</v>
+        <v>168000000</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -1625,15 +1630,15 @@
         <v>1</v>
       </c>
       <c r="D16" s="4">
-        <v>10000000</v>
+        <v>3500000</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>10000000</v>
+        <v>3500000</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>120000000</v>
+        <v>42000000</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1642,11 +1647,11 @@
       </c>
       <c r="E17" s="4">
         <f>SUBTOTAL(109,Table1[Total Cost/Month])</f>
-        <v>153711000</v>
+        <v>99361000</v>
       </c>
       <c r="F17" s="4">
         <f>SUBTOTAL(109,Table1[Total Annual Cost])</f>
-        <v>1844532000</v>
+        <v>1192332000</v>
       </c>
     </row>
   </sheetData>
@@ -1662,7 +1667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E35" sqref="E35:E44"/>
     </sheetView>
   </sheetViews>
@@ -1684,31 +1689,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="30" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="29"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="53"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="30"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1727,7 +1732,7 @@
       <c r="H3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="30"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="8" t="s">
         <v>23</v>
       </c>
@@ -1753,31 +1758,31 @@
       </c>
       <c r="C4" s="16">
         <f>$C21*$B$18</f>
-        <v>30000000</v>
+        <v>54000000</v>
       </c>
       <c r="D4" s="16">
         <f>$D21*$B$18</f>
-        <v>15000000</v>
+        <v>42000000</v>
       </c>
       <c r="E4" s="16">
         <f>$E21*$B$18</f>
-        <v>26400000</v>
+        <v>54000000</v>
       </c>
       <c r="F4" s="16">
         <f>$F21*$B$18</f>
-        <v>8400000</v>
+        <v>33180000</v>
       </c>
       <c r="G4" s="16">
         <f>$G21*$B$18</f>
-        <v>48000000</v>
+        <v>240000000</v>
       </c>
       <c r="H4" s="16">
         <f>$H21*$B$18</f>
-        <v>120000000</v>
+        <v>180000000</v>
       </c>
       <c r="I4" s="17">
         <f>SUM(C4:H4)</f>
-        <v>247800000</v>
+        <v>603180000</v>
       </c>
       <c r="J4" s="15" t="s">
         <v>32</v>
@@ -1804,55 +1809,55 @@
       </c>
       <c r="C5" s="16">
         <f t="shared" ref="C5:C13" si="0">$C22*$B$18</f>
-        <v>33000000</v>
+        <v>78000000</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" ref="D5:D13" si="1">$D22*$B$18</f>
-        <v>17400000</v>
+        <v>54000000</v>
       </c>
       <c r="E5" s="16">
         <f t="shared" ref="E5:E13" si="2">$E22*$B$18</f>
-        <v>30000000</v>
+        <v>66804000</v>
       </c>
       <c r="F5" s="16">
         <f t="shared" ref="F5:F13" si="3">$F22*$B$18</f>
-        <v>10800000</v>
+        <v>42804000</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" ref="G5:G13" si="4">$G22*$B$18</f>
-        <v>60000000</v>
+        <v>258000000</v>
       </c>
       <c r="H5" s="16">
         <f t="shared" ref="H5:H13" si="5">$H22*$B$18</f>
-        <v>156000000</v>
+        <v>192000000</v>
       </c>
       <c r="I5" s="17">
         <f t="shared" ref="I5:I13" si="6">SUM(C5:H5)</f>
-        <v>307200000</v>
+        <v>691608000</v>
       </c>
       <c r="J5" s="18">
         <f>(($C5-$C$4)/$C$4)</f>
-        <v>0.1</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="K5" s="18">
         <f>(($D5-$D$4)/$D$4)</f>
-        <v>0.16</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="L5" s="18">
         <f>(($E5-$E$4)/$E$4)</f>
-        <v>0.13636363636363635</v>
+        <v>0.23711111111111111</v>
       </c>
       <c r="M5" s="18">
         <f>(($F5-$F$4)/$F$4)</f>
-        <v>0.2857142857142857</v>
+        <v>0.29005424954792042</v>
       </c>
       <c r="N5" s="18">
         <f>(($G5-$G$4)/$G$4)</f>
-        <v>0.25</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O5" s="18">
         <f>(($H5-$H$4)/$H$4)</f>
-        <v>0.3</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -1861,55 +1866,55 @@
       </c>
       <c r="C6" s="16">
         <f t="shared" si="0"/>
-        <v>36000000</v>
+        <v>96000000</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="1"/>
-        <v>19200000</v>
+        <v>78000000</v>
       </c>
       <c r="E6" s="16">
         <f t="shared" si="2"/>
-        <v>31500000</v>
+        <v>81468000</v>
       </c>
       <c r="F6" s="16">
         <f t="shared" si="3"/>
-        <v>11400000</v>
+        <v>48120000</v>
       </c>
       <c r="G6" s="16">
         <f t="shared" si="4"/>
-        <v>67800000</v>
+        <v>294804000</v>
       </c>
       <c r="H6" s="16">
         <f t="shared" si="5"/>
-        <v>174300000</v>
+        <v>204000000</v>
       </c>
       <c r="I6" s="17">
         <f t="shared" si="6"/>
-        <v>340200000</v>
+        <v>802392000</v>
       </c>
       <c r="J6" s="18">
         <f t="shared" ref="J6:J13" si="7">(($C6-$C$4)/$C$4)</f>
-        <v>0.2</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K6" s="18">
         <f t="shared" ref="K6:K13" si="8">(($D6-$D$4)/$D$4)</f>
-        <v>0.28000000000000003</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="L6" s="18">
         <f t="shared" ref="L6:L13" si="9">(($E6-$E$4)/$E$4)</f>
-        <v>0.19318181818181818</v>
+        <v>0.50866666666666671</v>
       </c>
       <c r="M6" s="18">
         <f t="shared" ref="M6:M13" si="10">(($F6-$F$4)/$F$4)</f>
-        <v>0.35714285714285715</v>
+        <v>0.45027124773960214</v>
       </c>
       <c r="N6" s="18">
         <f t="shared" ref="N6:N13" si="11">(($G6-$G$4)/$G$4)</f>
-        <v>0.41249999999999998</v>
+        <v>0.22835</v>
       </c>
       <c r="O6" s="18">
         <f t="shared" ref="O6:O13" si="12">(($H6-$H$4)/$H$4)</f>
-        <v>0.45250000000000001</v>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -1918,55 +1923,55 @@
       </c>
       <c r="C7" s="16">
         <f t="shared" si="0"/>
-        <v>39000000</v>
+        <v>114816000</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="1"/>
-        <v>22200000</v>
+        <v>84000000</v>
       </c>
       <c r="E7" s="16">
         <f t="shared" si="2"/>
-        <v>33060000</v>
+        <v>95844000</v>
       </c>
       <c r="F7" s="16">
         <f t="shared" si="3"/>
-        <v>15000000</v>
+        <v>72000000</v>
       </c>
       <c r="G7" s="16">
         <f t="shared" si="4"/>
-        <v>72000000</v>
+        <v>312000000</v>
       </c>
       <c r="H7" s="16">
         <f t="shared" si="5"/>
-        <v>187824000</v>
+        <v>225180000</v>
       </c>
       <c r="I7" s="17">
         <f t="shared" si="6"/>
-        <v>369084000</v>
+        <v>903840000</v>
       </c>
       <c r="J7" s="18">
         <f t="shared" si="7"/>
-        <v>0.3</v>
+        <v>1.1262222222222222</v>
       </c>
       <c r="K7" s="18">
         <f t="shared" si="8"/>
-        <v>0.48</v>
+        <v>1</v>
       </c>
       <c r="L7" s="18">
         <f t="shared" si="9"/>
-        <v>0.25227272727272726</v>
+        <v>0.77488888888888885</v>
       </c>
       <c r="M7" s="18">
         <f t="shared" si="10"/>
-        <v>0.7857142857142857</v>
+        <v>1.1699819168173597</v>
       </c>
       <c r="N7" s="18">
         <f t="shared" si="11"/>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="O7" s="18">
         <f t="shared" si="12"/>
-        <v>0.56520000000000004</v>
+        <v>0.251</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -1975,55 +1980,55 @@
       </c>
       <c r="C8" s="16">
         <f t="shared" si="0"/>
-        <v>42000000</v>
+        <v>158808000</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="1"/>
-        <v>31200000</v>
+        <v>96000000</v>
       </c>
       <c r="E8" s="16">
         <f t="shared" si="2"/>
-        <v>38400000</v>
+        <v>117468000</v>
       </c>
       <c r="F8" s="16">
         <f t="shared" si="3"/>
-        <v>18000000</v>
+        <v>90780000</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="4"/>
-        <v>75000000</v>
+        <v>334680000</v>
       </c>
       <c r="H8" s="16">
         <f t="shared" si="5"/>
-        <v>196200000</v>
+        <v>235848000</v>
       </c>
       <c r="I8" s="17">
         <f t="shared" si="6"/>
-        <v>400800000</v>
+        <v>1033584000</v>
       </c>
       <c r="J8" s="18">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>1.9408888888888889</v>
       </c>
       <c r="K8" s="18">
         <f t="shared" si="8"/>
-        <v>1.08</v>
+        <v>1.2857142857142858</v>
       </c>
       <c r="L8" s="18">
         <f t="shared" si="9"/>
-        <v>0.45454545454545453</v>
+        <v>1.1753333333333333</v>
       </c>
       <c r="M8" s="18">
         <f t="shared" si="10"/>
-        <v>1.1428571428571428</v>
+        <v>1.7359855334538878</v>
       </c>
       <c r="N8" s="18">
         <f t="shared" si="11"/>
-        <v>0.5625</v>
+        <v>0.39450000000000002</v>
       </c>
       <c r="O8" s="18">
         <f t="shared" si="12"/>
-        <v>0.63500000000000001</v>
+        <v>0.31026666666666669</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -2032,55 +2037,55 @@
       </c>
       <c r="C9" s="16">
         <f t="shared" si="0"/>
-        <v>42600000</v>
+        <v>192000000</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="1"/>
-        <v>31800000</v>
+        <v>114000000</v>
       </c>
       <c r="E9" s="16">
         <f t="shared" si="2"/>
-        <v>39000000</v>
+        <v>132000000</v>
       </c>
       <c r="F9" s="16">
         <f t="shared" si="3"/>
-        <v>19800000</v>
+        <v>115884000</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="4"/>
-        <v>78000000</v>
+        <v>348000000</v>
       </c>
       <c r="H9" s="16">
         <f t="shared" si="5"/>
-        <v>200400000</v>
+        <v>252000000</v>
       </c>
       <c r="I9" s="17">
         <f t="shared" si="6"/>
-        <v>411600000</v>
+        <v>1153884000</v>
       </c>
       <c r="J9" s="18">
         <f t="shared" si="7"/>
-        <v>0.42</v>
+        <v>2.5555555555555554</v>
       </c>
       <c r="K9" s="18">
         <f t="shared" si="8"/>
-        <v>1.1200000000000001</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="L9" s="18">
         <f t="shared" si="9"/>
-        <v>0.47727272727272729</v>
+        <v>1.4444444444444444</v>
       </c>
       <c r="M9" s="18">
         <f t="shared" si="10"/>
-        <v>1.3571428571428572</v>
+        <v>2.4925858951175406</v>
       </c>
       <c r="N9" s="18">
         <f t="shared" si="11"/>
-        <v>0.625</v>
+        <v>0.45</v>
       </c>
       <c r="O9" s="18">
         <f t="shared" si="12"/>
-        <v>0.67</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -2089,55 +2094,55 @@
       </c>
       <c r="C10" s="16">
         <f t="shared" si="0"/>
-        <v>45000000</v>
+        <v>210552000</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="1"/>
-        <v>34200000</v>
+        <v>132000000</v>
       </c>
       <c r="E10" s="16">
         <f t="shared" si="2"/>
-        <v>41400000</v>
+        <v>150552000</v>
       </c>
       <c r="F10" s="16">
         <f t="shared" si="3"/>
-        <v>21420000</v>
+        <v>144000000</v>
       </c>
       <c r="G10" s="16">
         <f t="shared" si="4"/>
-        <v>78600000</v>
+        <v>372000000</v>
       </c>
       <c r="H10" s="16">
         <f t="shared" si="5"/>
-        <v>203424000</v>
+        <v>259848000</v>
       </c>
       <c r="I10" s="17">
         <f t="shared" si="6"/>
-        <v>424044000</v>
+        <v>1268952000</v>
       </c>
       <c r="J10" s="18">
         <f t="shared" si="7"/>
-        <v>0.5</v>
+        <v>2.899111111111111</v>
       </c>
       <c r="K10" s="18">
         <f t="shared" si="8"/>
-        <v>1.28</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="L10" s="18">
         <f t="shared" si="9"/>
-        <v>0.56818181818181823</v>
+        <v>1.788</v>
       </c>
       <c r="M10" s="18">
         <f t="shared" si="10"/>
-        <v>1.55</v>
+        <v>3.3399638336347195</v>
       </c>
       <c r="N10" s="18">
         <f t="shared" si="11"/>
-        <v>0.63749999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O10" s="18">
         <f t="shared" si="12"/>
-        <v>0.69520000000000004</v>
+        <v>0.44359999999999999</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -2146,55 +2151,55 @@
       </c>
       <c r="C11" s="16">
         <f t="shared" si="0"/>
-        <v>47400000</v>
+        <v>276000000</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="1"/>
-        <v>35580000</v>
+        <v>141216000</v>
       </c>
       <c r="E11" s="16">
         <f t="shared" si="2"/>
-        <v>42780000</v>
+        <v>165180000</v>
       </c>
       <c r="F11" s="16">
         <f t="shared" si="3"/>
-        <v>23040000</v>
+        <v>153204000</v>
       </c>
       <c r="G11" s="16">
         <f t="shared" si="4"/>
-        <v>79860000</v>
+        <v>384000000</v>
       </c>
       <c r="H11" s="16">
         <f t="shared" si="5"/>
-        <v>207000000</v>
+        <v>273036000</v>
       </c>
       <c r="I11" s="17">
         <f t="shared" si="6"/>
-        <v>435660000</v>
+        <v>1392636000</v>
       </c>
       <c r="J11" s="18">
         <f t="shared" si="7"/>
-        <v>0.57999999999999996</v>
+        <v>4.1111111111111107</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="8"/>
-        <v>1.3720000000000001</v>
+        <v>2.3622857142857141</v>
       </c>
       <c r="L11" s="18">
         <f t="shared" si="9"/>
-        <v>0.62045454545454548</v>
+        <v>2.0588888888888888</v>
       </c>
       <c r="M11" s="18">
         <f t="shared" si="10"/>
-        <v>1.7428571428571429</v>
+        <v>3.6173598553345387</v>
       </c>
       <c r="N11" s="18">
         <f t="shared" si="11"/>
-        <v>0.66374999999999995</v>
+        <v>0.6</v>
       </c>
       <c r="O11" s="18">
         <f t="shared" si="12"/>
-        <v>0.72499999999999998</v>
+        <v>0.5168666666666667</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
@@ -2203,55 +2208,55 @@
       </c>
       <c r="C12" s="16">
         <f t="shared" si="0"/>
-        <v>48696000</v>
+        <v>300000000</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="1"/>
-        <v>37824000</v>
+        <v>162552000</v>
       </c>
       <c r="E12" s="16">
         <f t="shared" si="2"/>
-        <v>44400000</v>
+        <v>188148000</v>
       </c>
       <c r="F12" s="16">
         <f t="shared" si="3"/>
-        <v>25500000</v>
+        <v>157872000</v>
       </c>
       <c r="G12" s="16">
         <f t="shared" si="4"/>
-        <v>82200000</v>
+        <v>390804000</v>
       </c>
       <c r="H12" s="16">
         <f t="shared" si="5"/>
-        <v>210300000</v>
+        <v>283848000</v>
       </c>
       <c r="I12" s="17">
         <f t="shared" si="6"/>
-        <v>448920000</v>
+        <v>1483224000</v>
       </c>
       <c r="J12" s="18">
         <f t="shared" si="7"/>
-        <v>0.62319999999999998</v>
+        <v>4.5555555555555554</v>
       </c>
       <c r="K12" s="18">
         <f t="shared" si="8"/>
-        <v>1.5216000000000001</v>
+        <v>2.8702857142857141</v>
       </c>
       <c r="L12" s="18">
         <f t="shared" si="9"/>
-        <v>0.68181818181818177</v>
+        <v>2.4842222222222223</v>
       </c>
       <c r="M12" s="18">
         <f t="shared" si="10"/>
-        <v>2.0357142857142856</v>
+        <v>3.7580470162748645</v>
       </c>
       <c r="N12" s="18">
         <f t="shared" si="11"/>
-        <v>0.71250000000000002</v>
+        <v>0.62834999999999996</v>
       </c>
       <c r="O12" s="18">
         <f t="shared" si="12"/>
-        <v>0.75249999999999995</v>
+        <v>0.5769333333333333</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -2260,55 +2265,55 @@
       </c>
       <c r="C13" s="16">
         <f t="shared" si="0"/>
-        <v>51000000</v>
+        <v>318540000</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="1"/>
-        <v>42300000</v>
+        <v>184140000</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="2"/>
-        <v>48000000</v>
+        <v>201108000</v>
       </c>
       <c r="F13" s="16">
         <f t="shared" si="3"/>
-        <v>30540000</v>
+        <v>178512000</v>
       </c>
       <c r="G13" s="16">
         <f t="shared" si="4"/>
-        <v>84600000</v>
+        <v>420000000</v>
       </c>
       <c r="H13" s="16">
         <f t="shared" si="5"/>
-        <v>217500000</v>
+        <v>294804000</v>
       </c>
       <c r="I13" s="17">
         <f t="shared" si="6"/>
-        <v>473940000</v>
+        <v>1597104000</v>
       </c>
       <c r="J13" s="18">
         <f t="shared" si="7"/>
-        <v>0.7</v>
+        <v>4.8988888888888891</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="8"/>
-        <v>1.82</v>
+        <v>3.3842857142857143</v>
       </c>
       <c r="L13" s="18">
         <f t="shared" si="9"/>
-        <v>0.81818181818181823</v>
+        <v>2.7242222222222221</v>
       </c>
       <c r="M13" s="18">
         <f t="shared" si="10"/>
-        <v>2.6357142857142857</v>
+        <v>4.380108499095841</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" si="11"/>
-        <v>0.76249999999999996</v>
+        <v>0.75</v>
       </c>
       <c r="O13" s="18">
         <f t="shared" si="12"/>
-        <v>0.8125</v>
+        <v>0.63780000000000003</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -2323,7 +2328,7 @@
       </c>
       <c r="I14" s="20">
         <f>SUM(I4:I13)</f>
-        <v>3859248000</v>
+        <v>10930404000</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -2398,28 +2403,28 @@
       <c r="N18" s="14"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="30" t="s">
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="33"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="7" t="s">
         <v>23</v>
       </c>
@@ -2462,22 +2467,22 @@
         <v>1</v>
       </c>
       <c r="C21" s="16">
-        <v>2500000</v>
+        <v>4500000</v>
       </c>
       <c r="D21" s="16">
-        <v>1250000</v>
+        <v>3500000</v>
       </c>
       <c r="E21" s="16">
-        <v>2200000</v>
+        <v>4500000</v>
       </c>
       <c r="F21" s="16">
-        <v>700000</v>
+        <v>2765000</v>
       </c>
       <c r="G21" s="16">
-        <v>4000000</v>
+        <v>20000000</v>
       </c>
       <c r="H21" s="16">
-        <v>10000000</v>
+        <v>15000000</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -2491,22 +2496,22 @@
         <v>2</v>
       </c>
       <c r="C22" s="17">
-        <v>2750000</v>
+        <v>6500000</v>
       </c>
       <c r="D22" s="17">
-        <v>1450000</v>
+        <v>4500000</v>
       </c>
       <c r="E22" s="17">
-        <v>2500000</v>
+        <v>5567000</v>
       </c>
       <c r="F22" s="17">
-        <v>900000</v>
+        <v>3567000</v>
       </c>
       <c r="G22" s="17">
-        <v>5000000</v>
+        <v>21500000</v>
       </c>
       <c r="H22" s="17">
-        <v>13000000</v>
+        <v>16000000</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -2520,22 +2525,22 @@
         <v>3</v>
       </c>
       <c r="C23" s="17">
-        <v>3000000</v>
+        <v>8000000</v>
       </c>
       <c r="D23" s="17">
-        <v>1600000</v>
+        <v>6500000</v>
       </c>
       <c r="E23" s="17">
-        <v>2625000</v>
+        <v>6789000</v>
       </c>
       <c r="F23" s="17">
-        <v>950000</v>
+        <v>4010000</v>
       </c>
       <c r="G23" s="17">
-        <v>5650000</v>
+        <v>24567000</v>
       </c>
       <c r="H23" s="17">
-        <v>14525000</v>
+        <v>17000000</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -2549,22 +2554,22 @@
         <v>4</v>
       </c>
       <c r="C24" s="17">
-        <v>3250000</v>
+        <v>9568000</v>
       </c>
       <c r="D24" s="17">
-        <v>1850000</v>
+        <v>7000000</v>
       </c>
       <c r="E24" s="17">
-        <v>2755000</v>
+        <v>7987000</v>
       </c>
       <c r="F24" s="17">
-        <v>1250000</v>
+        <v>6000000</v>
       </c>
       <c r="G24" s="17">
-        <v>6000000</v>
+        <v>26000000</v>
       </c>
       <c r="H24" s="17">
-        <v>15652000</v>
+        <v>18765000</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -2578,22 +2583,22 @@
         <v>5</v>
       </c>
       <c r="C25" s="17">
-        <v>3500000</v>
+        <v>13234000</v>
       </c>
       <c r="D25" s="17">
-        <v>2600000</v>
+        <v>8000000</v>
       </c>
       <c r="E25" s="17">
-        <v>3200000</v>
+        <v>9789000</v>
       </c>
       <c r="F25" s="17">
-        <v>1500000</v>
+        <v>7565000</v>
       </c>
       <c r="G25" s="17">
-        <v>6250000</v>
+        <v>27890000</v>
       </c>
       <c r="H25" s="17">
-        <v>16350000</v>
+        <v>19654000</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
@@ -2607,22 +2612,22 @@
         <v>6</v>
       </c>
       <c r="C26" s="17">
-        <v>3550000</v>
+        <v>16000000</v>
       </c>
       <c r="D26" s="17">
-        <v>2650000</v>
+        <v>9500000</v>
       </c>
       <c r="E26" s="17">
-        <v>3250000</v>
+        <v>11000000</v>
       </c>
       <c r="F26" s="17">
-        <v>1650000</v>
+        <v>9657000</v>
       </c>
       <c r="G26" s="17">
-        <v>6500000</v>
+        <v>29000000</v>
       </c>
       <c r="H26" s="17">
-        <v>16700000</v>
+        <v>21000000</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
@@ -2636,22 +2641,22 @@
         <v>7</v>
       </c>
       <c r="C27" s="17">
-        <v>3750000</v>
+        <v>17546000</v>
       </c>
       <c r="D27" s="17">
-        <v>2850000</v>
+        <v>11000000</v>
       </c>
       <c r="E27" s="17">
-        <v>3450000</v>
+        <v>12546000</v>
       </c>
       <c r="F27" s="17">
-        <v>1785000</v>
+        <v>12000000</v>
       </c>
       <c r="G27" s="17">
-        <v>6550000</v>
+        <v>31000000</v>
       </c>
       <c r="H27" s="17">
-        <v>16952000</v>
+        <v>21654000</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -2665,22 +2670,22 @@
         <v>8</v>
       </c>
       <c r="C28" s="17">
-        <v>3950000</v>
+        <v>23000000</v>
       </c>
       <c r="D28" s="17">
-        <v>2965000</v>
+        <v>11768000</v>
       </c>
       <c r="E28" s="17">
-        <v>3565000</v>
+        <v>13765000</v>
       </c>
       <c r="F28" s="17">
-        <v>1920000</v>
+        <v>12767000</v>
       </c>
       <c r="G28" s="17">
-        <v>6655000</v>
+        <v>32000000</v>
       </c>
       <c r="H28" s="17">
-        <v>17250000</v>
+        <v>22753000</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
@@ -2694,22 +2699,22 @@
         <v>9</v>
       </c>
       <c r="C29" s="17">
-        <v>4058000</v>
+        <v>25000000</v>
       </c>
       <c r="D29" s="17">
-        <v>3152000</v>
+        <v>13546000</v>
       </c>
       <c r="E29" s="17">
-        <v>3700000</v>
+        <v>15679000</v>
       </c>
       <c r="F29" s="17">
-        <v>2125000</v>
+        <v>13156000</v>
       </c>
       <c r="G29" s="17">
-        <v>6850000</v>
+        <v>32567000</v>
       </c>
       <c r="H29" s="17">
-        <v>17525000</v>
+        <v>23654000</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -2723,22 +2728,22 @@
         <v>10</v>
       </c>
       <c r="C30" s="17">
-        <v>4250000</v>
+        <v>26545000</v>
       </c>
       <c r="D30" s="17">
-        <v>3525000</v>
+        <v>15345000</v>
       </c>
       <c r="E30" s="17">
-        <v>4000000</v>
+        <v>16759000</v>
       </c>
       <c r="F30" s="17">
-        <v>2545000</v>
+        <v>14876000</v>
       </c>
       <c r="G30" s="17">
-        <v>7050000</v>
+        <v>35000000</v>
       </c>
       <c r="H30" s="17">
-        <v>18125000</v>
+        <v>24567000</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -2748,34 +2753,34 @@
       <c r="N30" s="6"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="32"/>
-      <c r="E33" s="33" t="s">
+      <c r="D33" s="55"/>
+      <c r="E33" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="28" t="s">
+      <c r="F33" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="29"/>
+      <c r="G33" s="53"/>
       <c r="H33" s="21"/>
       <c r="I33" s="21"/>
       <c r="J33" s="21"/>
       <c r="K33" s="21"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="34"/>
+      <c r="E34" s="57"/>
       <c r="F34" s="8" t="s">
         <v>35</v>
       </c>
@@ -2793,14 +2798,14 @@
       </c>
       <c r="C35" s="16">
         <f>$I4</f>
-        <v>247800000</v>
+        <v>603180000</v>
       </c>
       <c r="D35" s="16">
-        <v>76250000</v>
+        <v>300000000</v>
       </c>
       <c r="E35" s="17">
         <f>SUM(C35,D35)</f>
-        <v>324050000</v>
+        <v>903180000</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>32</v>
@@ -2819,22 +2824,22 @@
       </c>
       <c r="C36" s="16">
         <f t="shared" ref="C36:C44" si="13">$I5</f>
-        <v>307200000</v>
+        <v>691608000</v>
       </c>
       <c r="D36" s="16">
-        <v>92252000</v>
+        <v>350000000</v>
       </c>
       <c r="E36" s="17">
         <f t="shared" ref="E36:E44" si="14">SUM(C36,D36)</f>
-        <v>399452000</v>
+        <v>1041608000</v>
       </c>
       <c r="F36" s="18">
         <f>($C36-$C35)/$C35</f>
-        <v>0.23970944309927361</v>
+        <v>0.14660300407838456</v>
       </c>
       <c r="G36" s="18">
         <f>($D36-$D35)/$D35</f>
-        <v>0.20986229508196722</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
@@ -2847,22 +2852,22 @@
       </c>
       <c r="C37" s="16">
         <f t="shared" si="13"/>
-        <v>340200000</v>
+        <v>802392000</v>
       </c>
       <c r="D37" s="16">
-        <v>95000000</v>
+        <v>385000000</v>
       </c>
       <c r="E37" s="17">
         <f t="shared" si="14"/>
-        <v>435200000</v>
+        <v>1187392000</v>
       </c>
       <c r="F37" s="18">
         <f t="shared" ref="F37:F44" si="15">($C37-$C36)/$C36</f>
-        <v>0.107421875</v>
+        <v>0.1601832251795815</v>
       </c>
       <c r="G37" s="18">
         <f>($D37-$D36)/$D36</f>
-        <v>2.9787972076486147E-2</v>
+        <v>0.1</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -2875,22 +2880,22 @@
       </c>
       <c r="C38" s="16">
         <f t="shared" si="13"/>
-        <v>369084000</v>
+        <v>903840000</v>
       </c>
       <c r="D38" s="16">
-        <v>98152000</v>
+        <v>387000000</v>
       </c>
       <c r="E38" s="17">
         <f t="shared" si="14"/>
-        <v>467236000</v>
+        <v>1290840000</v>
       </c>
       <c r="F38" s="18">
         <f>($C38-$C37)/$C37</f>
-        <v>8.4902998236331573E-2</v>
+        <v>0.12643196841444082</v>
       </c>
       <c r="G38" s="18">
         <f>($D38-$D37)/$D37</f>
-        <v>3.3178947368421051E-2</v>
+        <v>5.1948051948051948E-3</v>
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
@@ -2903,22 +2908,22 @@
       </c>
       <c r="C39" s="16">
         <f t="shared" si="13"/>
-        <v>400800000</v>
+        <v>1033584000</v>
       </c>
       <c r="D39" s="16">
-        <v>100545000</v>
+        <v>397000000</v>
       </c>
       <c r="E39" s="17">
         <f t="shared" si="14"/>
-        <v>501345000</v>
+        <v>1430584000</v>
       </c>
       <c r="F39" s="18">
         <f>($C39-$C38)/$C38</f>
-        <v>8.5931657833989011E-2</v>
+        <v>0.14354753053637812</v>
       </c>
       <c r="G39" s="18">
         <f t="shared" ref="G39:G44" si="16">($D39-$D38)/$D38</f>
-        <v>2.4380552612274838E-2</v>
+        <v>2.5839793281653745E-2</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
@@ -2931,22 +2936,22 @@
       </c>
       <c r="C40" s="16">
         <f t="shared" si="13"/>
-        <v>411600000</v>
+        <v>1153884000</v>
       </c>
       <c r="D40" s="16">
-        <v>101205000</v>
+        <v>412000000</v>
       </c>
       <c r="E40" s="17">
         <f t="shared" si="14"/>
-        <v>512805000</v>
+        <v>1565884000</v>
       </c>
       <c r="F40" s="18">
         <f t="shared" si="15"/>
-        <v>2.6946107784431138E-2</v>
+        <v>0.11639112060558213</v>
       </c>
       <c r="G40" s="18">
         <f>($D40-$D39)/$D39</f>
-        <v>6.5642249738922867E-3</v>
+        <v>3.7783375314861464E-2</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
@@ -2959,22 +2964,22 @@
       </c>
       <c r="C41" s="16">
         <f t="shared" si="13"/>
-        <v>424044000</v>
+        <v>1268952000</v>
       </c>
       <c r="D41" s="16">
-        <v>102000000</v>
+        <v>465000000</v>
       </c>
       <c r="E41" s="17">
         <f t="shared" si="14"/>
-        <v>526044000</v>
+        <v>1733952000</v>
       </c>
       <c r="F41" s="18">
         <f>($C41-$C40)/$C40</f>
-        <v>3.0233236151603497E-2</v>
+        <v>9.972232910760527E-2</v>
       </c>
       <c r="G41" s="18">
         <f t="shared" si="16"/>
-        <v>7.8553431154587232E-3</v>
+        <v>0.12864077669902912</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23"/>
@@ -2987,22 +2992,22 @@
       </c>
       <c r="C42" s="16">
         <f t="shared" si="13"/>
-        <v>435660000</v>
+        <v>1392636000</v>
       </c>
       <c r="D42" s="16">
-        <v>110250000</v>
+        <v>487000000</v>
       </c>
       <c r="E42" s="17">
         <f t="shared" si="14"/>
-        <v>545910000</v>
+        <v>1879636000</v>
       </c>
       <c r="F42" s="18">
         <f t="shared" si="15"/>
-        <v>2.7393383705464527E-2</v>
+        <v>9.7469407826300758E-2</v>
       </c>
       <c r="G42" s="18">
         <f t="shared" si="16"/>
-        <v>8.0882352941176475E-2</v>
+        <v>4.7311827956989246E-2</v>
       </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
@@ -3015,22 +3020,22 @@
       </c>
       <c r="C43" s="16">
         <f t="shared" si="13"/>
-        <v>448920000</v>
+        <v>1483224000</v>
       </c>
       <c r="D43" s="16">
-        <v>116585000</v>
+        <v>505460000</v>
       </c>
       <c r="E43" s="17">
         <f t="shared" si="14"/>
-        <v>565505000</v>
+        <v>1988684000</v>
       </c>
       <c r="F43" s="18">
         <f t="shared" si="15"/>
-        <v>3.0436578983611073E-2</v>
+        <v>6.5047866061196183E-2</v>
       </c>
       <c r="G43" s="18">
         <f t="shared" si="16"/>
-        <v>5.7460317460317462E-2</v>
+        <v>3.7905544147843945E-2</v>
       </c>
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
@@ -3043,22 +3048,22 @@
       </c>
       <c r="C44" s="16">
         <f t="shared" si="13"/>
-        <v>473940000</v>
+        <v>1597104000</v>
       </c>
       <c r="D44" s="16">
-        <v>120000000</v>
+        <v>515000000</v>
       </c>
       <c r="E44" s="17">
         <f t="shared" si="14"/>
-        <v>593940000</v>
+        <v>2112104000</v>
       </c>
       <c r="F44" s="18">
         <f t="shared" si="15"/>
-        <v>5.5733761026463512E-2</v>
+        <v>7.6778692901409359E-2</v>
       </c>
       <c r="G44" s="18">
         <f t="shared" si="16"/>
-        <v>2.9291932924475704E-2</v>
+        <v>1.88738970442765E-2</v>
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
@@ -3073,7 +3078,7 @@
       </c>
       <c r="E45" s="20">
         <f>SUM(E35:E44)</f>
-        <v>4871487000</v>
+        <v>15133864000</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -3108,7 +3113,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3278,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,122 +3322,220 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>60500000</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+        <f>SUBTOTAL(109,Table6[Total])</f>
+        <v>67400000</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E3" s="27">
+        <v>903180000</v>
+      </c>
       <c r="F3" s="27">
-        <v>324050000</v>
-      </c>
-      <c r="G3" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>-356552000</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="4">
+        <f>SUBTOTAL(109,Table6[Total])</f>
+        <v>67400000</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E4" s="27">
+        <v>1041608000</v>
+      </c>
       <c r="F4" s="27">
-        <v>399452000</v>
-      </c>
-      <c r="G4" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>-218124000</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="4">
+        <f>SUBTOTAL(109,Table6[Total])</f>
+        <v>67400000</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E5" s="27">
+        <v>1187392000</v>
+      </c>
       <c r="F5" s="27">
-        <v>435200000</v>
-      </c>
-      <c r="G5" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>-72340000</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E6" s="27">
+        <v>1290840000</v>
+      </c>
       <c r="F6" s="27">
-        <v>467236000</v>
-      </c>
-      <c r="G6" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>31108000</v>
+      </c>
+      <c r="G6" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>31108000</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E7" s="27">
+        <v>1430584000</v>
+      </c>
       <c r="F7" s="27">
-        <v>501345000</v>
-      </c>
-      <c r="G7" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>170852000</v>
+      </c>
+      <c r="G7" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>170852000</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E8" s="27">
+        <v>1565884000</v>
+      </c>
       <c r="F8" s="27">
-        <v>512805000</v>
-      </c>
-      <c r="G8" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>306152000</v>
+      </c>
+      <c r="G8" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>306152000</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E9" s="27">
+        <v>1733952000</v>
+      </c>
       <c r="F9" s="27">
-        <v>526044000</v>
-      </c>
-      <c r="G9" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>474220000</v>
+      </c>
+      <c r="G9" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>474220000</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E10" s="27">
+        <v>1879636000</v>
+      </c>
       <c r="F10" s="27">
-        <v>545910000</v>
-      </c>
-      <c r="G10" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>619904000</v>
+      </c>
+      <c r="G10" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>619904000</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E11" s="27">
+        <v>1988684000</v>
+      </c>
       <c r="F11" s="27">
-        <v>565505000</v>
-      </c>
-      <c r="G11" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>728952000</v>
+      </c>
+      <c r="G11" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>728952000</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1192332000</v>
+      </c>
+      <c r="E12" s="27">
+        <v>2112104000</v>
+      </c>
       <c r="F12" s="27">
-        <v>593940000</v>
-      </c>
-      <c r="G12" s="4"/>
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>852372000</v>
+      </c>
+      <c r="G12" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>852372000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3446,8 +3549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3457,426 +3560,426 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="28" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="49"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="49"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="39"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="59"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="49"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="59"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="49"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="59"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="49"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="57"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J15" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="38" t="s">
+      <c r="N15" s="28" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="48"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="38"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="50"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="40"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="49"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="39"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="49"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="39"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="59"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="49"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="59"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="49"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="59"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="49"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="57"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
#20161117 -> Break event point analysis updated
</commit_message>
<xml_diff>
--- a/PPT/Financial Analysis.xlsx
+++ b/PPT/Financial Analysis.xlsx
@@ -602,7 +602,10 @@
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="43">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;Rp&quot;\ #,##0;\-&quot;Rp&quot;\ #,##0"/>
     </dxf>
@@ -989,27 +992,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F17" totalsRowCount="1" headerRowDxfId="41" headerRowCellStyle="Accent3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F17" totalsRowCount="1" headerRowDxfId="42" headerRowCellStyle="Accent3">
   <autoFilter ref="B2:F16"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Quantity"/>
-    <tableColumn id="3" name="Cost/Month" dataDxfId="40"/>
-    <tableColumn id="4" name="Total Cost/Month" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="6"/>
-    <tableColumn id="5" name="Total Annual Cost" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Cost/Month" dataDxfId="41"/>
+    <tableColumn id="4" name="Total Cost/Month" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="7"/>
+    <tableColumn id="5" name="Total Annual Cost" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:E11" totalsRowCount="1" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B2:E11" totalsRowCount="1" headerRowDxfId="38">
   <autoFilter ref="B2:E10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Quantity"/>
-    <tableColumn id="3" name="@" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="4" name="Total" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33">
+    <tableColumn id="3" name="@" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="4" name="Total" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>Table6[[#This Row],[@]]*Table6[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1018,63 +1021,68 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B2:G12" totalsRowShown="0">
-  <autoFilter ref="B2:G12"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B2:H12" totalsRowShown="0">
+  <autoFilter ref="B2:H12"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="Tahun Ke-"/>
-    <tableColumn id="2" name="Sunk Cost Remaining" dataDxfId="4">
+    <tableColumn id="2" name="Sunk Cost Remaining" dataDxfId="5">
       <calculatedColumnFormula>SUBTOTAL(109,Table6[Total])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Total Cost" dataDxfId="3"/>
-    <tableColumn id="4" name="Total Revenue" dataDxfId="1"/>
-    <tableColumn id="5" name="Profit" dataDxfId="0">
+    <tableColumn id="3" name="Total Cost" dataDxfId="4"/>
+    <tableColumn id="4" name="Total Revenue" dataDxfId="3"/>
+    <tableColumn id="5" name="Profit" dataDxfId="2">
       <calculatedColumnFormula>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Net Profit After Sunk Cost" dataDxfId="2"/>
+    <tableColumn id="6" name="Net Profit After Sunk Cost" dataDxfId="1">
+      <calculatedColumnFormula>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Total Profit" dataDxfId="0">
+      <calculatedColumnFormula>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:N12" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B3:N12" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="B3:N12"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Task/Month"/>
-    <tableColumn id="2" name="1" dataDxfId="31"/>
-    <tableColumn id="3" name="2" dataDxfId="30"/>
-    <tableColumn id="4" name="3" dataDxfId="29"/>
-    <tableColumn id="5" name="4" dataDxfId="28"/>
-    <tableColumn id="6" name="5" dataDxfId="27"/>
-    <tableColumn id="7" name="6" dataDxfId="26"/>
-    <tableColumn id="8" name="7" dataDxfId="25"/>
-    <tableColumn id="9" name="8" dataDxfId="24"/>
-    <tableColumn id="10" name="9" dataDxfId="23"/>
-    <tableColumn id="11" name="10" dataDxfId="22"/>
-    <tableColumn id="12" name="11" dataDxfId="21"/>
-    <tableColumn id="13" name="12" dataDxfId="20"/>
+    <tableColumn id="2" name="1" dataDxfId="32"/>
+    <tableColumn id="3" name="2" dataDxfId="31"/>
+    <tableColumn id="4" name="3" dataDxfId="30"/>
+    <tableColumn id="5" name="4" dataDxfId="29"/>
+    <tableColumn id="6" name="5" dataDxfId="28"/>
+    <tableColumn id="7" name="6" dataDxfId="27"/>
+    <tableColumn id="8" name="7" dataDxfId="26"/>
+    <tableColumn id="9" name="8" dataDxfId="25"/>
+    <tableColumn id="10" name="9" dataDxfId="24"/>
+    <tableColumn id="11" name="10" dataDxfId="23"/>
+    <tableColumn id="12" name="11" dataDxfId="22"/>
+    <tableColumn id="13" name="12" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B15:N24" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="B15:N24" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="B15:N24"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Task/Month"/>
-    <tableColumn id="2" name="1" dataDxfId="18"/>
-    <tableColumn id="3" name="2" dataDxfId="17"/>
-    <tableColumn id="4" name="3" dataDxfId="16"/>
-    <tableColumn id="5" name="4" dataDxfId="15"/>
-    <tableColumn id="6" name="5" dataDxfId="14"/>
-    <tableColumn id="7" name="6" dataDxfId="13"/>
-    <tableColumn id="8" name="7" dataDxfId="12"/>
-    <tableColumn id="9" name="8" dataDxfId="11"/>
-    <tableColumn id="10" name="9" dataDxfId="10"/>
-    <tableColumn id="11" name="10" dataDxfId="9"/>
-    <tableColumn id="12" name="11" dataDxfId="8"/>
-    <tableColumn id="13" name="12" dataDxfId="7"/>
+    <tableColumn id="2" name="1" dataDxfId="19"/>
+    <tableColumn id="3" name="2" dataDxfId="18"/>
+    <tableColumn id="4" name="3" dataDxfId="17"/>
+    <tableColumn id="5" name="4" dataDxfId="16"/>
+    <tableColumn id="6" name="5" dataDxfId="15"/>
+    <tableColumn id="7" name="6" dataDxfId="14"/>
+    <tableColumn id="8" name="7" dataDxfId="13"/>
+    <tableColumn id="9" name="8" dataDxfId="12"/>
+    <tableColumn id="10" name="9" dataDxfId="11"/>
+    <tableColumn id="11" name="10" dataDxfId="10"/>
+    <tableColumn id="12" name="11" dataDxfId="9"/>
+    <tableColumn id="13" name="12" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1346,7 +1354,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E35" sqref="E35:E44"/>
     </sheetView>
   </sheetViews>
@@ -1758,19 +1766,19 @@
       </c>
       <c r="C4" s="16">
         <f>$C21*$B$18</f>
-        <v>54000000</v>
+        <v>180000000</v>
       </c>
       <c r="D4" s="16">
         <f>$D21*$B$18</f>
-        <v>42000000</v>
+        <v>144000000</v>
       </c>
       <c r="E4" s="16">
         <f>$E21*$B$18</f>
-        <v>54000000</v>
+        <v>137472000</v>
       </c>
       <c r="F4" s="16">
         <f>$F21*$B$18</f>
-        <v>33180000</v>
+        <v>120000000</v>
       </c>
       <c r="G4" s="16">
         <f>$G21*$B$18</f>
@@ -1782,7 +1790,7 @@
       </c>
       <c r="I4" s="17">
         <f>SUM(C4:H4)</f>
-        <v>603180000</v>
+        <v>1001472000</v>
       </c>
       <c r="J4" s="15" t="s">
         <v>32</v>
@@ -1809,19 +1817,19 @@
       </c>
       <c r="C5" s="16">
         <f t="shared" ref="C5:C13" si="0">$C22*$B$18</f>
-        <v>78000000</v>
+        <v>198000000</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" ref="D5:D13" si="1">$D22*$B$18</f>
-        <v>54000000</v>
+        <v>156000000</v>
       </c>
       <c r="E5" s="16">
         <f t="shared" ref="E5:E13" si="2">$E22*$B$18</f>
-        <v>66804000</v>
+        <v>148140000</v>
       </c>
       <c r="F5" s="16">
         <f t="shared" ref="F5:F13" si="3">$F22*$B$18</f>
-        <v>42804000</v>
+        <v>144000000</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" ref="G5:G13" si="4">$G22*$B$18</f>
@@ -1833,23 +1841,23 @@
       </c>
       <c r="I5" s="17">
         <f t="shared" ref="I5:I13" si="6">SUM(C5:H5)</f>
-        <v>691608000</v>
+        <v>1096140000</v>
       </c>
       <c r="J5" s="18">
         <f>(($C5-$C$4)/$C$4)</f>
-        <v>0.44444444444444442</v>
+        <v>0.1</v>
       </c>
       <c r="K5" s="18">
         <f>(($D5-$D$4)/$D$4)</f>
-        <v>0.2857142857142857</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="L5" s="18">
         <f>(($E5-$E$4)/$E$4)</f>
-        <v>0.23711111111111111</v>
+        <v>7.7601256983240219E-2</v>
       </c>
       <c r="M5" s="18">
         <f>(($F5-$F$4)/$F$4)</f>
-        <v>0.29005424954792042</v>
+        <v>0.2</v>
       </c>
       <c r="N5" s="18">
         <f>(($G5-$G$4)/$G$4)</f>
@@ -1866,19 +1874,19 @@
       </c>
       <c r="C6" s="16">
         <f t="shared" si="0"/>
-        <v>96000000</v>
+        <v>210000000</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="1"/>
-        <v>78000000</v>
+        <v>185256000</v>
       </c>
       <c r="E6" s="16">
         <f t="shared" si="2"/>
-        <v>81468000</v>
+        <v>161472000</v>
       </c>
       <c r="F6" s="16">
         <f t="shared" si="3"/>
-        <v>48120000</v>
+        <v>151884000</v>
       </c>
       <c r="G6" s="16">
         <f t="shared" si="4"/>
@@ -1890,23 +1898,23 @@
       </c>
       <c r="I6" s="17">
         <f t="shared" si="6"/>
-        <v>802392000</v>
+        <v>1207416000</v>
       </c>
       <c r="J6" s="18">
         <f t="shared" ref="J6:J13" si="7">(($C6-$C$4)/$C$4)</f>
-        <v>0.77777777777777779</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K6" s="18">
         <f t="shared" ref="K6:K13" si="8">(($D6-$D$4)/$D$4)</f>
-        <v>0.8571428571428571</v>
+        <v>0.28649999999999998</v>
       </c>
       <c r="L6" s="18">
         <f t="shared" ref="L6:L13" si="9">(($E6-$E$4)/$E$4)</f>
-        <v>0.50866666666666671</v>
+        <v>0.17458100558659218</v>
       </c>
       <c r="M6" s="18">
         <f t="shared" ref="M6:M13" si="10">(($F6-$F$4)/$F$4)</f>
-        <v>0.45027124773960214</v>
+        <v>0.26569999999999999</v>
       </c>
       <c r="N6" s="18">
         <f t="shared" ref="N6:N13" si="11">(($G6-$G$4)/$G$4)</f>
@@ -1923,19 +1931,19 @@
       </c>
       <c r="C7" s="16">
         <f t="shared" si="0"/>
-        <v>114816000</v>
+        <v>222000000</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="1"/>
-        <v>84000000</v>
+        <v>201048000</v>
       </c>
       <c r="E7" s="16">
         <f t="shared" si="2"/>
-        <v>95844000</v>
+        <v>174000000</v>
       </c>
       <c r="F7" s="16">
         <f t="shared" si="3"/>
-        <v>72000000</v>
+        <v>162804000</v>
       </c>
       <c r="G7" s="16">
         <f t="shared" si="4"/>
@@ -1947,23 +1955,23 @@
       </c>
       <c r="I7" s="17">
         <f t="shared" si="6"/>
-        <v>903840000</v>
+        <v>1297032000</v>
       </c>
       <c r="J7" s="18">
         <f t="shared" si="7"/>
-        <v>1.1262222222222222</v>
+        <v>0.23333333333333334</v>
       </c>
       <c r="K7" s="18">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0.39616666666666667</v>
       </c>
       <c r="L7" s="18">
         <f t="shared" si="9"/>
-        <v>0.77488888888888885</v>
+        <v>0.26571229050279327</v>
       </c>
       <c r="M7" s="18">
         <f t="shared" si="10"/>
-        <v>1.1699819168173597</v>
+        <v>0.35670000000000002</v>
       </c>
       <c r="N7" s="18">
         <f t="shared" si="11"/>
@@ -1980,19 +1988,19 @@
       </c>
       <c r="C8" s="16">
         <f t="shared" si="0"/>
-        <v>158808000</v>
+        <v>234720000</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="1"/>
-        <v>96000000</v>
+        <v>209472000</v>
       </c>
       <c r="E8" s="16">
         <f t="shared" si="2"/>
-        <v>117468000</v>
+        <v>186000000</v>
       </c>
       <c r="F8" s="16">
         <f t="shared" si="3"/>
-        <v>90780000</v>
+        <v>174804000</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="4"/>
@@ -2004,23 +2012,23 @@
       </c>
       <c r="I8" s="17">
         <f t="shared" si="6"/>
-        <v>1033584000</v>
+        <v>1375524000</v>
       </c>
       <c r="J8" s="18">
         <f t="shared" si="7"/>
-        <v>1.9408888888888889</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="K8" s="18">
         <f t="shared" si="8"/>
-        <v>1.2857142857142858</v>
+        <v>0.45466666666666666</v>
       </c>
       <c r="L8" s="18">
         <f t="shared" si="9"/>
-        <v>1.1753333333333333</v>
+        <v>0.35300279329608941</v>
       </c>
       <c r="M8" s="18">
         <f t="shared" si="10"/>
-        <v>1.7359855334538878</v>
+        <v>0.45669999999999999</v>
       </c>
       <c r="N8" s="18">
         <f t="shared" si="11"/>
@@ -2037,19 +2045,19 @@
       </c>
       <c r="C9" s="16">
         <f t="shared" si="0"/>
-        <v>192000000</v>
+        <v>252000000</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="1"/>
-        <v>114000000</v>
+        <v>225214800</v>
       </c>
       <c r="E9" s="16">
         <f t="shared" si="2"/>
-        <v>132000000</v>
+        <v>198000000</v>
       </c>
       <c r="F9" s="16">
         <f t="shared" si="3"/>
-        <v>115884000</v>
+        <v>185472000</v>
       </c>
       <c r="G9" s="16">
         <f t="shared" si="4"/>
@@ -2061,23 +2069,23 @@
       </c>
       <c r="I9" s="17">
         <f t="shared" si="6"/>
-        <v>1153884000</v>
+        <v>1460686800</v>
       </c>
       <c r="J9" s="18">
         <f t="shared" si="7"/>
-        <v>2.5555555555555554</v>
+        <v>0.4</v>
       </c>
       <c r="K9" s="18">
         <f t="shared" si="8"/>
-        <v>1.7142857142857142</v>
+        <v>0.56399166666666667</v>
       </c>
       <c r="L9" s="18">
         <f t="shared" si="9"/>
-        <v>1.4444444444444444</v>
+        <v>0.4402932960893855</v>
       </c>
       <c r="M9" s="18">
         <f t="shared" si="10"/>
-        <v>2.4925858951175406</v>
+        <v>0.54559999999999997</v>
       </c>
       <c r="N9" s="18">
         <f t="shared" si="11"/>
@@ -2094,19 +2102,19 @@
       </c>
       <c r="C10" s="16">
         <f t="shared" si="0"/>
-        <v>210552000</v>
+        <v>259884000</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="1"/>
-        <v>132000000</v>
+        <v>233472000</v>
       </c>
       <c r="E10" s="16">
         <f t="shared" si="2"/>
-        <v>150552000</v>
+        <v>210000000</v>
       </c>
       <c r="F10" s="16">
         <f t="shared" si="3"/>
-        <v>144000000</v>
+        <v>197472000</v>
       </c>
       <c r="G10" s="16">
         <f t="shared" si="4"/>
@@ -2118,23 +2126,23 @@
       </c>
       <c r="I10" s="17">
         <f t="shared" si="6"/>
-        <v>1268952000</v>
+        <v>1532676000</v>
       </c>
       <c r="J10" s="18">
         <f t="shared" si="7"/>
-        <v>2.899111111111111</v>
+        <v>0.44379999999999997</v>
       </c>
       <c r="K10" s="18">
         <f t="shared" si="8"/>
-        <v>2.1428571428571428</v>
+        <v>0.62133333333333329</v>
       </c>
       <c r="L10" s="18">
         <f t="shared" si="9"/>
-        <v>1.788</v>
+        <v>0.52758379888268159</v>
       </c>
       <c r="M10" s="18">
         <f t="shared" si="10"/>
-        <v>3.3399638336347195</v>
+        <v>0.64559999999999995</v>
       </c>
       <c r="N10" s="18">
         <f t="shared" si="11"/>
@@ -2151,19 +2159,19 @@
       </c>
       <c r="C11" s="16">
         <f t="shared" si="0"/>
-        <v>276000000</v>
+        <v>282552000</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="1"/>
-        <v>141216000</v>
+        <v>252000000</v>
       </c>
       <c r="E11" s="16">
         <f t="shared" si="2"/>
-        <v>165180000</v>
+        <v>222000000</v>
       </c>
       <c r="F11" s="16">
         <f t="shared" si="3"/>
-        <v>153204000</v>
+        <v>211893600</v>
       </c>
       <c r="G11" s="16">
         <f t="shared" si="4"/>
@@ -2175,23 +2183,23 @@
       </c>
       <c r="I11" s="17">
         <f t="shared" si="6"/>
-        <v>1392636000</v>
+        <v>1625481600</v>
       </c>
       <c r="J11" s="18">
         <f t="shared" si="7"/>
-        <v>4.1111111111111107</v>
+        <v>0.56973333333333331</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="8"/>
-        <v>2.3622857142857141</v>
+        <v>0.75</v>
       </c>
       <c r="L11" s="18">
         <f t="shared" si="9"/>
-        <v>2.0588888888888888</v>
+        <v>0.61487430167597767</v>
       </c>
       <c r="M11" s="18">
         <f t="shared" si="10"/>
-        <v>3.6173598553345387</v>
+        <v>0.76578000000000002</v>
       </c>
       <c r="N11" s="18">
         <f t="shared" si="11"/>
@@ -2208,19 +2216,19 @@
       </c>
       <c r="C12" s="16">
         <f t="shared" si="0"/>
-        <v>300000000</v>
+        <v>311844000</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="1"/>
-        <v>162552000</v>
+        <v>264000000</v>
       </c>
       <c r="E12" s="16">
         <f t="shared" si="2"/>
-        <v>188148000</v>
+        <v>234000000</v>
       </c>
       <c r="F12" s="16">
         <f t="shared" si="3"/>
-        <v>157872000</v>
+        <v>224136000</v>
       </c>
       <c r="G12" s="16">
         <f t="shared" si="4"/>
@@ -2232,23 +2240,23 @@
       </c>
       <c r="I12" s="17">
         <f t="shared" si="6"/>
-        <v>1483224000</v>
+        <v>1708632000</v>
       </c>
       <c r="J12" s="18">
         <f t="shared" si="7"/>
-        <v>4.5555555555555554</v>
+        <v>0.73246666666666671</v>
       </c>
       <c r="K12" s="18">
         <f t="shared" si="8"/>
-        <v>2.8702857142857141</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="L12" s="18">
         <f t="shared" si="9"/>
-        <v>2.4842222222222223</v>
+        <v>0.70216480446927376</v>
       </c>
       <c r="M12" s="18">
         <f t="shared" si="10"/>
-        <v>3.7580470162748645</v>
+        <v>0.86780000000000002</v>
       </c>
       <c r="N12" s="18">
         <f t="shared" si="11"/>
@@ -2265,19 +2273,19 @@
       </c>
       <c r="C13" s="16">
         <f t="shared" si="0"/>
-        <v>318540000</v>
+        <v>318804000</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="1"/>
-        <v>184140000</v>
+        <v>268140000</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="2"/>
-        <v>201108000</v>
+        <v>252000000</v>
       </c>
       <c r="F13" s="16">
         <f t="shared" si="3"/>
-        <v>178512000</v>
+        <v>237468000</v>
       </c>
       <c r="G13" s="16">
         <f t="shared" si="4"/>
@@ -2289,23 +2297,23 @@
       </c>
       <c r="I13" s="17">
         <f t="shared" si="6"/>
-        <v>1597104000</v>
+        <v>1791216000</v>
       </c>
       <c r="J13" s="18">
         <f t="shared" si="7"/>
-        <v>4.8988888888888891</v>
+        <v>0.77113333333333334</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="8"/>
-        <v>3.3842857142857143</v>
+        <v>0.86208333333333331</v>
       </c>
       <c r="L13" s="18">
         <f t="shared" si="9"/>
-        <v>2.7242222222222221</v>
+        <v>0.83310055865921784</v>
       </c>
       <c r="M13" s="18">
         <f t="shared" si="10"/>
-        <v>4.380108499095841</v>
+        <v>0.97889999999999999</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" si="11"/>
@@ -2328,7 +2336,7 @@
       </c>
       <c r="I14" s="20">
         <f>SUM(I4:I13)</f>
-        <v>10930404000</v>
+        <v>14096276400</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -2467,16 +2475,16 @@
         <v>1</v>
       </c>
       <c r="C21" s="16">
-        <v>4500000</v>
+        <v>15000000</v>
       </c>
       <c r="D21" s="16">
-        <v>3500000</v>
+        <v>12000000</v>
       </c>
       <c r="E21" s="16">
-        <v>4500000</v>
+        <v>11456000</v>
       </c>
       <c r="F21" s="16">
-        <v>2765000</v>
+        <v>10000000</v>
       </c>
       <c r="G21" s="16">
         <v>20000000</v>
@@ -2495,17 +2503,17 @@
       <c r="B22" s="10">
         <v>2</v>
       </c>
-      <c r="C22" s="17">
-        <v>6500000</v>
+      <c r="C22" s="16">
+        <v>16500000</v>
       </c>
       <c r="D22" s="17">
-        <v>4500000</v>
+        <v>13000000</v>
       </c>
       <c r="E22" s="17">
-        <v>5567000</v>
+        <v>12345000</v>
       </c>
       <c r="F22" s="17">
-        <v>3567000</v>
+        <v>12000000</v>
       </c>
       <c r="G22" s="17">
         <v>21500000</v>
@@ -2524,17 +2532,17 @@
       <c r="B23" s="9">
         <v>3</v>
       </c>
-      <c r="C23" s="17">
-        <v>8000000</v>
+      <c r="C23" s="16">
+        <v>17500000</v>
       </c>
       <c r="D23" s="17">
-        <v>6500000</v>
+        <v>15438000</v>
       </c>
       <c r="E23" s="17">
-        <v>6789000</v>
+        <v>13456000</v>
       </c>
       <c r="F23" s="17">
-        <v>4010000</v>
+        <v>12657000</v>
       </c>
       <c r="G23" s="17">
         <v>24567000</v>
@@ -2553,17 +2561,17 @@
       <c r="B24" s="10">
         <v>4</v>
       </c>
-      <c r="C24" s="17">
-        <v>9568000</v>
+      <c r="C24" s="16">
+        <v>18500000</v>
       </c>
       <c r="D24" s="17">
-        <v>7000000</v>
+        <v>16754000</v>
       </c>
       <c r="E24" s="17">
-        <v>7987000</v>
+        <v>14500000</v>
       </c>
       <c r="F24" s="17">
-        <v>6000000</v>
+        <v>13567000</v>
       </c>
       <c r="G24" s="17">
         <v>26000000</v>
@@ -2582,17 +2590,17 @@
       <c r="B25" s="9">
         <v>5</v>
       </c>
-      <c r="C25" s="17">
-        <v>13234000</v>
+      <c r="C25" s="16">
+        <v>19560000</v>
       </c>
       <c r="D25" s="17">
-        <v>8000000</v>
+        <v>17456000</v>
       </c>
       <c r="E25" s="17">
-        <v>9789000</v>
+        <v>15500000</v>
       </c>
       <c r="F25" s="17">
-        <v>7565000</v>
+        <v>14567000</v>
       </c>
       <c r="G25" s="17">
         <v>27890000</v>
@@ -2611,17 +2619,17 @@
       <c r="B26" s="10">
         <v>6</v>
       </c>
-      <c r="C26" s="17">
-        <v>16000000</v>
+      <c r="C26" s="16">
+        <v>21000000</v>
       </c>
       <c r="D26" s="17">
-        <v>9500000</v>
+        <v>18767900</v>
       </c>
       <c r="E26" s="17">
-        <v>11000000</v>
+        <v>16500000</v>
       </c>
       <c r="F26" s="17">
-        <v>9657000</v>
+        <v>15456000</v>
       </c>
       <c r="G26" s="17">
         <v>29000000</v>
@@ -2640,17 +2648,17 @@
       <c r="B27" s="9">
         <v>7</v>
       </c>
-      <c r="C27" s="17">
-        <v>17546000</v>
+      <c r="C27" s="16">
+        <v>21657000</v>
       </c>
       <c r="D27" s="17">
-        <v>11000000</v>
+        <v>19456000</v>
       </c>
       <c r="E27" s="17">
-        <v>12546000</v>
+        <v>17500000</v>
       </c>
       <c r="F27" s="17">
-        <v>12000000</v>
+        <v>16456000</v>
       </c>
       <c r="G27" s="17">
         <v>31000000</v>
@@ -2669,17 +2677,17 @@
       <c r="B28" s="10">
         <v>8</v>
       </c>
-      <c r="C28" s="17">
-        <v>23000000</v>
+      <c r="C28" s="16">
+        <v>23546000</v>
       </c>
       <c r="D28" s="17">
-        <v>11768000</v>
+        <v>21000000</v>
       </c>
       <c r="E28" s="17">
-        <v>13765000</v>
+        <v>18500000</v>
       </c>
       <c r="F28" s="17">
-        <v>12767000</v>
+        <v>17657800</v>
       </c>
       <c r="G28" s="17">
         <v>32000000</v>
@@ -2698,17 +2706,17 @@
       <c r="B29" s="9">
         <v>9</v>
       </c>
-      <c r="C29" s="17">
-        <v>25000000</v>
+      <c r="C29" s="16">
+        <v>25987000</v>
       </c>
       <c r="D29" s="17">
-        <v>13546000</v>
+        <v>22000000</v>
       </c>
       <c r="E29" s="17">
-        <v>15679000</v>
+        <v>19500000</v>
       </c>
       <c r="F29" s="17">
-        <v>13156000</v>
+        <v>18678000</v>
       </c>
       <c r="G29" s="17">
         <v>32567000</v>
@@ -2727,17 +2735,17 @@
       <c r="B30" s="10">
         <v>10</v>
       </c>
-      <c r="C30" s="17">
-        <v>26545000</v>
+      <c r="C30" s="16">
+        <v>26567000</v>
       </c>
       <c r="D30" s="17">
-        <v>15345000</v>
+        <v>22345000</v>
       </c>
       <c r="E30" s="17">
-        <v>16759000</v>
+        <v>21000000</v>
       </c>
       <c r="F30" s="17">
-        <v>14876000</v>
+        <v>19789000</v>
       </c>
       <c r="G30" s="17">
         <v>35000000</v>
@@ -2798,14 +2806,14 @@
       </c>
       <c r="C35" s="16">
         <f>$I4</f>
-        <v>603180000</v>
+        <v>1001472000</v>
       </c>
       <c r="D35" s="16">
-        <v>300000000</v>
+        <v>750000000</v>
       </c>
       <c r="E35" s="17">
         <f>SUM(C35,D35)</f>
-        <v>903180000</v>
+        <v>1751472000</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>32</v>
@@ -2824,22 +2832,22 @@
       </c>
       <c r="C36" s="16">
         <f t="shared" ref="C36:C44" si="13">$I5</f>
-        <v>691608000</v>
+        <v>1096140000</v>
       </c>
       <c r="D36" s="16">
-        <v>350000000</v>
+        <v>976000000</v>
       </c>
       <c r="E36" s="17">
         <f t="shared" ref="E36:E44" si="14">SUM(C36,D36)</f>
-        <v>1041608000</v>
+        <v>2072140000</v>
       </c>
       <c r="F36" s="18">
         <f>($C36-$C35)/$C35</f>
-        <v>0.14660300407838456</v>
+        <v>9.4528853527607357E-2</v>
       </c>
       <c r="G36" s="18">
         <f>($D36-$D35)/$D35</f>
-        <v>0.16666666666666666</v>
+        <v>0.30133333333333334</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
@@ -2852,22 +2860,22 @@
       </c>
       <c r="C37" s="16">
         <f t="shared" si="13"/>
-        <v>802392000</v>
+        <v>1207416000</v>
       </c>
       <c r="D37" s="16">
-        <v>385000000</v>
+        <v>1567000000</v>
       </c>
       <c r="E37" s="17">
         <f t="shared" si="14"/>
-        <v>1187392000</v>
+        <v>2774416000</v>
       </c>
       <c r="F37" s="18">
         <f t="shared" ref="F37:F44" si="15">($C37-$C36)/$C36</f>
-        <v>0.1601832251795815</v>
+        <v>0.10151622967869067</v>
       </c>
       <c r="G37" s="18">
         <f>($D37-$D36)/$D36</f>
-        <v>0.1</v>
+        <v>0.60553278688524592</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -2880,22 +2888,22 @@
       </c>
       <c r="C38" s="16">
         <f t="shared" si="13"/>
-        <v>903840000</v>
+        <v>1297032000</v>
       </c>
       <c r="D38" s="16">
-        <v>387000000</v>
+        <v>1998000000</v>
       </c>
       <c r="E38" s="17">
         <f t="shared" si="14"/>
-        <v>1290840000</v>
+        <v>3295032000</v>
       </c>
       <c r="F38" s="18">
         <f>($C38-$C37)/$C37</f>
-        <v>0.12643196841444082</v>
+        <v>7.4221312290047511E-2</v>
       </c>
       <c r="G38" s="18">
         <f>($D38-$D37)/$D37</f>
-        <v>5.1948051948051948E-3</v>
+        <v>0.2750478621569879</v>
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
@@ -2908,22 +2916,22 @@
       </c>
       <c r="C39" s="16">
         <f t="shared" si="13"/>
-        <v>1033584000</v>
+        <v>1375524000</v>
       </c>
       <c r="D39" s="16">
-        <v>397000000</v>
+        <v>2300000000</v>
       </c>
       <c r="E39" s="17">
         <f t="shared" si="14"/>
-        <v>1430584000</v>
+        <v>3675524000</v>
       </c>
       <c r="F39" s="18">
         <f>($C39-$C38)/$C38</f>
-        <v>0.14354753053637812</v>
+        <v>6.0516625649945414E-2</v>
       </c>
       <c r="G39" s="18">
         <f t="shared" ref="G39:G44" si="16">($D39-$D38)/$D38</f>
-        <v>2.5839793281653745E-2</v>
+        <v>0.15115115115115116</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
@@ -2936,22 +2944,22 @@
       </c>
       <c r="C40" s="16">
         <f t="shared" si="13"/>
-        <v>1153884000</v>
+        <v>1460686800</v>
       </c>
       <c r="D40" s="16">
-        <v>412000000</v>
+        <v>2567000000</v>
       </c>
       <c r="E40" s="17">
         <f t="shared" si="14"/>
-        <v>1565884000</v>
+        <v>4027686800</v>
       </c>
       <c r="F40" s="18">
         <f t="shared" si="15"/>
-        <v>0.11639112060558213</v>
+        <v>6.191298734155129E-2</v>
       </c>
       <c r="G40" s="18">
         <f>($D40-$D39)/$D39</f>
-        <v>3.7783375314861464E-2</v>
+        <v>0.11608695652173913</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
@@ -2964,22 +2972,22 @@
       </c>
       <c r="C41" s="16">
         <f t="shared" si="13"/>
-        <v>1268952000</v>
+        <v>1532676000</v>
       </c>
       <c r="D41" s="16">
-        <v>465000000</v>
+        <v>2879000000</v>
       </c>
       <c r="E41" s="17">
         <f t="shared" si="14"/>
-        <v>1733952000</v>
+        <v>4411676000</v>
       </c>
       <c r="F41" s="18">
         <f>($C41-$C40)/$C40</f>
-        <v>9.972232910760527E-2</v>
+        <v>4.9284487269960951E-2</v>
       </c>
       <c r="G41" s="18">
         <f t="shared" si="16"/>
-        <v>0.12864077669902912</v>
+        <v>0.12154265679781846</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23"/>
@@ -2992,22 +3000,22 @@
       </c>
       <c r="C42" s="16">
         <f t="shared" si="13"/>
-        <v>1392636000</v>
+        <v>1625481600</v>
       </c>
       <c r="D42" s="16">
-        <v>487000000</v>
+        <v>3240000000</v>
       </c>
       <c r="E42" s="17">
         <f t="shared" si="14"/>
-        <v>1879636000</v>
+        <v>4865481600</v>
       </c>
       <c r="F42" s="18">
         <f t="shared" si="15"/>
-        <v>9.7469407826300758E-2</v>
+        <v>6.0551349404570826E-2</v>
       </c>
       <c r="G42" s="18">
         <f t="shared" si="16"/>
-        <v>4.7311827956989246E-2</v>
+        <v>0.12539076068079194</v>
       </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
@@ -3020,22 +3028,22 @@
       </c>
       <c r="C43" s="16">
         <f t="shared" si="13"/>
-        <v>1483224000</v>
+        <v>1708632000</v>
       </c>
       <c r="D43" s="16">
-        <v>505460000</v>
+        <v>3456000000</v>
       </c>
       <c r="E43" s="17">
         <f t="shared" si="14"/>
-        <v>1988684000</v>
+        <v>5164632000</v>
       </c>
       <c r="F43" s="18">
         <f t="shared" si="15"/>
-        <v>6.5047866061196183E-2</v>
+        <v>5.1154316357687468E-2</v>
       </c>
       <c r="G43" s="18">
         <f t="shared" si="16"/>
-        <v>3.7905544147843945E-2</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
@@ -3048,22 +3056,22 @@
       </c>
       <c r="C44" s="16">
         <f t="shared" si="13"/>
-        <v>1597104000</v>
+        <v>1791216000</v>
       </c>
       <c r="D44" s="16">
-        <v>515000000</v>
+        <v>3765000000</v>
       </c>
       <c r="E44" s="17">
         <f t="shared" si="14"/>
-        <v>2112104000</v>
+        <v>5556216000</v>
       </c>
       <c r="F44" s="18">
         <f t="shared" si="15"/>
-        <v>7.6778692901409359E-2</v>
+        <v>4.8333403564957231E-2</v>
       </c>
       <c r="G44" s="18">
         <f t="shared" si="16"/>
-        <v>1.88738970442765E-2</v>
+        <v>8.9409722222222224E-2</v>
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
@@ -3078,7 +3086,7 @@
       </c>
       <c r="E45" s="20">
         <f>SUM(E35:E44)</f>
-        <v>15133864000</v>
+        <v>37594276400</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
@@ -3281,10 +3289,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B2" sqref="B2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,9 +3303,10 @@
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -3316,8 +3325,11 @@
       <c r="G2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -3329,61 +3341,74 @@
         <v>1192332000</v>
       </c>
       <c r="E3" s="27">
-        <v>903180000</v>
+        <v>1751472000</v>
       </c>
       <c r="F3" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>-356552000</v>
-      </c>
-      <c r="G3" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>491740000</v>
+      </c>
+      <c r="G3" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>491740000</v>
+      </c>
+      <c r="H3" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>491740000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
-        <f>SUBTOTAL(109,Table6[Total])</f>
-        <v>67400000</v>
+      <c r="C4" s="60" t="s">
+        <v>32</v>
       </c>
       <c r="D4" s="4">
         <v>1192332000</v>
       </c>
       <c r="E4" s="27">
-        <v>1041608000</v>
+        <v>2072140000</v>
       </c>
       <c r="F4" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>-218124000</v>
-      </c>
-      <c r="G4" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+        <v>812408000</v>
+      </c>
+      <c r="G4" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>812408000</v>
+      </c>
+      <c r="H4" s="27">
+        <f>$F4+$F3</f>
+        <v>1304148000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
-        <f>SUBTOTAL(109,Table6[Total])</f>
-        <v>67400000</v>
+      <c r="C5" s="60" t="s">
+        <v>32</v>
       </c>
       <c r="D5" s="4">
         <v>1192332000</v>
       </c>
       <c r="E5" s="27">
-        <v>1187392000</v>
+        <v>2774416000</v>
       </c>
       <c r="F5" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>-72340000</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>1514684000</v>
+      </c>
+      <c r="G5" s="27">
+        <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
+        <v>1514684000</v>
+      </c>
+      <c r="H5" s="27">
+        <f>$F5+$F4</f>
+        <v>2327092000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -3394,18 +3419,22 @@
         <v>1192332000</v>
       </c>
       <c r="E6" s="27">
-        <v>1290840000</v>
+        <v>3295032000</v>
       </c>
       <c r="F6" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>31108000</v>
+        <v>2035300000</v>
       </c>
       <c r="G6" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>31108000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>2035300000</v>
+      </c>
+      <c r="H6" s="27">
+        <f>$F6+$F5</f>
+        <v>3549984000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -3416,18 +3445,22 @@
         <v>1192332000</v>
       </c>
       <c r="E7" s="27">
-        <v>1430584000</v>
+        <v>3675524000</v>
       </c>
       <c r="F7" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>170852000</v>
+        <v>2415792000</v>
       </c>
       <c r="G7" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>170852000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+        <v>2415792000</v>
+      </c>
+      <c r="H7" s="27">
+        <f t="shared" ref="H5:H12" si="0">$F7+$F6</f>
+        <v>4451092000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -3438,18 +3471,22 @@
         <v>1192332000</v>
       </c>
       <c r="E8" s="27">
-        <v>1565884000</v>
+        <v>4027686800</v>
       </c>
       <c r="F8" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>306152000</v>
+        <v>2767954800</v>
       </c>
       <c r="G8" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>306152000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <v>2767954800</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="0"/>
+        <v>5183746800</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
@@ -3460,18 +3497,22 @@
         <v>1192332000</v>
       </c>
       <c r="E9" s="27">
-        <v>1733952000</v>
+        <v>4411676000</v>
       </c>
       <c r="F9" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>474220000</v>
+        <v>3151944000</v>
       </c>
       <c r="G9" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>474220000</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+        <v>3151944000</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="0"/>
+        <v>5919898800</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
@@ -3482,18 +3523,22 @@
         <v>1192332000</v>
       </c>
       <c r="E10" s="27">
-        <v>1879636000</v>
+        <v>4865481600</v>
       </c>
       <c r="F10" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>619904000</v>
+        <v>3605749600</v>
       </c>
       <c r="G10" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>619904000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <v>3605749600</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="0"/>
+        <v>6757693600</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
@@ -3504,18 +3549,22 @@
         <v>1192332000</v>
       </c>
       <c r="E11" s="27">
-        <v>1988684000</v>
+        <v>5164632000</v>
       </c>
       <c r="F11" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>728952000</v>
+        <v>3904900000</v>
       </c>
       <c r="G11" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>728952000</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>3904900000</v>
+      </c>
+      <c r="H11" s="27">
+        <f t="shared" si="0"/>
+        <v>7510649600</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -3526,15 +3575,19 @@
         <v>1192332000</v>
       </c>
       <c r="E12" s="27">
-        <v>2112104000</v>
+        <v>5556216000</v>
       </c>
       <c r="F12" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>852372000</v>
+        <v>4296484000</v>
       </c>
       <c r="G12" s="27">
         <f>Table7[[#This Row],[Total Revenue]]-Table7[[#This Row],[Total Cost]]-$C$3</f>
-        <v>852372000</v>
+        <v>4296484000</v>
+      </c>
+      <c r="H12" s="27">
+        <f t="shared" si="0"/>
+        <v>8201384000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>